<commit_message>
added BHANSA to ACE factsheets list
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8C611C-2613-42D1-B026-F0F7D96BADFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3541A0E7-2DD6-44AB-BC60-AD0F1B382AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>year_data</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>UkSATSE</t>
+  </si>
+  <si>
+    <t>BHANSA</t>
   </si>
 </sst>
 </file>
@@ -341,6 +344,7 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1422,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,166 +1469,171 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
202309 September full release
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8C611C-2613-42D1-B026-F0F7D96BADFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3541A0E7-2DD6-44AB-BC60-AD0F1B382AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>year_data</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>UkSATSE</t>
+  </si>
+  <si>
+    <t>BHANSA</t>
   </si>
 </sst>
 </file>
@@ -341,6 +344,7 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1422,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,166 +1469,171 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replaced HCAA by HASP in ACE menu
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3541A0E7-2DD6-44AB-BC60-AD0F1B382AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62206CB-11D9-4D90-B928-E996E1F53A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -129,9 +129,6 @@
     <t>Fintraffic ANS</t>
   </si>
   <si>
-    <t>HCAA</t>
-  </si>
-  <si>
     <t>HungaroControl</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>BHANSA</t>
+  </si>
+  <si>
+    <t>HASP</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:O7"/>
     </sheetView>
   </sheetViews>
@@ -1428,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1524,117 +1524,117 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
202310 October full release
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3541A0E7-2DD6-44AB-BC60-AD0F1B382AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62206CB-11D9-4D90-B928-E996E1F53A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -129,9 +129,6 @@
     <t>Fintraffic ANS</t>
   </si>
   <si>
-    <t>HCAA</t>
-  </si>
-  <si>
     <t>HungaroControl</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>BHANSA</t>
+  </si>
+  <si>
+    <t>HASP</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:O7"/>
     </sheetView>
   </sheetViews>
@@ -1428,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1524,117 +1524,117 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update ACE landing page
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62206CB-11D9-4D90-B928-E996E1F53A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E99A6FF-C4F5-49C7-BBF3-848343A8D0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -1084,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,278 +1139,278 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B2">
-        <v>662.65521777397339</v>
+        <v>470.15663229742336</v>
       </c>
       <c r="C2">
-        <v>7934149622.8315115</v>
+        <v>8921474338.786293</v>
       </c>
       <c r="D2">
-        <v>11973269.673306623</v>
+        <v>18975536.504061323</v>
       </c>
       <c r="E2">
-        <v>0.60100490180918753</v>
+        <v>0.8836954720487562</v>
       </c>
       <c r="F2">
-        <v>125.59558798069767</v>
+        <v>133.16679170159205</v>
       </c>
       <c r="G2">
-        <v>453.6792383724395</v>
+        <v>319.46355316139619</v>
       </c>
       <c r="H2">
-        <v>-0.25256080837562622</v>
+        <v>-0.34650568426651729</v>
       </c>
       <c r="I2">
-        <v>-4.9472216575946248E-2</v>
+        <v>3.4409572293988999E-2</v>
       </c>
       <c r="J2">
-        <v>0.27171252735398754</v>
+        <v>0.58288993092918751</v>
       </c>
       <c r="K2">
-        <v>0.2512561872807817</v>
+        <v>0.46856790462369879</v>
       </c>
       <c r="L2">
-        <v>-8.2366239265637464E-2</v>
+        <v>-2.3420464129504381E-2</v>
       </c>
       <c r="M2">
-        <v>-0.24589697880793293</v>
+        <v>-0.35179038408891561</v>
       </c>
       <c r="N2">
-        <v>94.696214877447176</v>
+        <v>96.927408574309311</v>
       </c>
       <c r="O2">
-        <v>61.682595642255713</v>
+        <v>93.290786227371314</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B3">
-        <v>886.56739598288459</v>
+        <v>719.45022470427932</v>
       </c>
       <c r="C3">
-        <v>8347099118.1873665</v>
+        <v>8624702030.7452507</v>
       </c>
       <c r="D3">
-        <v>9415075.668255806</v>
+        <v>11987906.507764762</v>
       </c>
       <c r="E3">
-        <v>0.48032122271881494</v>
+        <v>0.60173960582040065</v>
       </c>
       <c r="F3">
-        <v>136.86897033974233</v>
+        <v>136.36041593160243</v>
       </c>
       <c r="G3">
-        <v>601.61440230709434</v>
+        <v>492.83988592544631</v>
       </c>
       <c r="H3">
-        <v>1.2158530364034017</v>
+        <v>-0.25294214079289401</v>
       </c>
       <c r="I3">
-        <v>-4.0858436680157206E-2</v>
+        <v>-4.9983832135574113E-2</v>
       </c>
       <c r="J3">
-        <v>-0.56714567818240957</v>
+        <v>0.27167682684274408</v>
       </c>
       <c r="K3">
-        <v>-0.50703672301460312</v>
+        <v>0.25122106103595776</v>
       </c>
       <c r="L3">
-        <v>8.6351440285316938E-2</v>
+        <v>-8.2189450562490274E-2</v>
       </c>
       <c r="M3">
-        <v>1.2216481187552026</v>
+        <v>-0.246553986261564</v>
       </c>
       <c r="N3">
-        <v>99.624878439982297</v>
+        <v>93.703124149707335</v>
       </c>
       <c r="O3">
-        <v>48.503568468100852</v>
+        <v>58.937001496122846</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B4">
-        <v>400.10207419797615</v>
+        <v>963.04485099436852</v>
       </c>
       <c r="C4">
-        <v>8702676890.8813076</v>
+        <v>9078479211.7096443</v>
       </c>
       <c r="D4">
-        <v>21751141.651355449</v>
+        <v>9426849.8526687324</v>
       </c>
       <c r="E4">
-        <v>0.97435497762857415</v>
+        <v>0.48092189666483548</v>
       </c>
       <c r="F4">
-        <v>125.98958795856649</v>
+        <v>148.57141924896419</v>
       </c>
       <c r="G4">
-        <v>270.79644036706452</v>
+        <v>654.11439829654353</v>
       </c>
       <c r="H4">
-        <v>-2.4701332369039264E-3</v>
+        <v>1.2134441067149506</v>
       </c>
       <c r="I4">
-        <v>1.4080583617405162E-2</v>
+        <v>-4.188692214530354E-2</v>
       </c>
       <c r="J4">
-        <v>1.6591700565332212E-2</v>
+        <v>-0.56713924921435421</v>
       </c>
       <c r="K4">
-        <v>1.0170212828736203E-2</v>
+        <v>-0.50702940127839669</v>
       </c>
       <c r="L4">
-        <v>6.3459591994674547E-3</v>
+        <v>8.47184440380222E-2</v>
       </c>
       <c r="M4">
-        <v>-1.8406972416513678E-3</v>
+        <v>1.2196723111014927</v>
       </c>
       <c r="N4">
-        <v>103.86879502453654</v>
+        <v>98.633188907032832</v>
       </c>
       <c r="O4">
-        <v>112.05517889813467</v>
+        <v>46.345895633286567</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B5">
-        <v>401.09282692083707</v>
+        <v>435.08885002913263</v>
       </c>
       <c r="C5">
-        <v>8581839581.0689087</v>
+        <v>9475373441.3449364</v>
       </c>
       <c r="D5">
-        <v>21396143.249309942</v>
+        <v>21778019.456739664</v>
       </c>
       <c r="E5">
-        <v>0.96454534617500731</v>
+        <v>0.97555898447490952</v>
       </c>
       <c r="F5">
-        <v>125.19510493070321</v>
+        <v>136.96772657048723</v>
       </c>
       <c r="G5">
-        <v>271.29581382324051</v>
+        <v>294.68962379043467</v>
       </c>
       <c r="H5">
-        <v>-3.6094428167074533E-2</v>
+        <v>-2.4139029120445743E-3</v>
       </c>
       <c r="I5">
-        <v>1.5247568031038439E-2</v>
+        <v>1.411651830421401E-2</v>
       </c>
       <c r="J5">
-        <v>5.3264549659654881E-2</v>
+        <v>1.6570420602805447E-2</v>
       </c>
       <c r="K5">
-        <v>4.9168678899710994E-2</v>
+        <v>1.0149067284991542E-2</v>
       </c>
       <c r="L5">
-        <v>-4.4919207430094144E-4</v>
+        <v>6.1435452387501588E-3</v>
       </c>
       <c r="M5">
-        <v>-3.0643239613244E-2</v>
+        <v>-1.673078925594762E-3</v>
       </c>
       <c r="N5">
-        <v>102.4265691529347</v>
+        <v>102.94524851688867</v>
       </c>
       <c r="O5">
-        <v>110.22633652804777</v>
+        <v>107.06883345086935</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B6">
-        <v>416.11215729164684</v>
+        <v>436.14165363691069</v>
       </c>
       <c r="C6">
-        <v>8452952611.0684977</v>
+        <v>9343476090.0941372</v>
       </c>
       <c r="D6">
-        <v>20314120.755534545</v>
+        <v>21423030.825376313</v>
       </c>
       <c r="E6">
-        <v>0.91934249046259153</v>
+        <v>0.96575744716267398</v>
       </c>
       <c r="F6">
-        <v>125.25136685198848</v>
+        <v>136.13139717353735</v>
       </c>
       <c r="G6">
-        <v>279.87199853539818</v>
+        <v>295.18348906517315</v>
       </c>
       <c r="H6">
-        <v>-3.5965088317736371E-2</v>
+        <v>-3.6186849785866837E-2</v>
       </c>
       <c r="I6">
-        <v>8.8826841671714174E-3</v>
+        <v>1.5122489958370178E-2</v>
       </c>
       <c r="J6">
-        <v>4.6520900790457453E-2</v>
+        <v>5.3235774727536489E-2</v>
       </c>
       <c r="K6">
-        <v>4.2159218877963145E-2</v>
+        <v>4.91400158657882E-2</v>
       </c>
       <c r="L6">
-        <v>1.1290411509541576E-2</v>
+        <v>-3.0022649526117995E-4</v>
       </c>
       <c r="M6">
-        <v>-3.9023886136794417E-2</v>
+        <v>-3.087473276982311E-2</v>
       </c>
       <c r="N6">
-        <v>100.88826841671714</v>
+        <v>101.51224899583701</v>
       </c>
       <c r="O6">
-        <v>104.65209007904575</v>
+        <v>105.32357747275366</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B7">
-        <v>431.63598356155103</v>
+        <v>452.51681152100053</v>
       </c>
       <c r="C7">
-        <v>8378528786.0762281</v>
+        <v>9204284391.8050823</v>
       </c>
       <c r="D7">
-        <v>19411098.947179075</v>
+        <v>20340204.291786686</v>
       </c>
       <c r="E7">
-        <v>0.88215166532077338</v>
+        <v>0.92052293550703623</v>
       </c>
       <c r="F7">
-        <v>123.85301534207885</v>
+        <v>136.17227969982335</v>
       </c>
       <c r="G7">
-        <v>291.23720610524748</v>
+        <v>304.58754822152844</v>
       </c>
       <c r="H7">
-        <v>-1.9200542076866833E-2</v>
+        <v>-3.5869632351568481E-2</v>
       </c>
       <c r="I7">
-        <v>6.5683161127729761E-3</v>
+        <v>8.9638823037501147E-3</v>
       </c>
       <c r="J7">
-        <v>2.6273320179240223E-2</v>
+        <v>4.6501506600886477E-2</v>
       </c>
       <c r="K7">
-        <v>1.8151797095498079E-2</v>
+        <v>4.2139905519349652E-2</v>
       </c>
       <c r="L7">
-        <v>1.6252900049103625E-2</v>
+        <v>1.1321105465380787E-2</v>
       </c>
       <c r="M7">
-        <v>-2.7344259646731262E-2</v>
+        <v>-3.8898520130888015E-2</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1428,7 +1428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
202312 December full release
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62206CB-11D9-4D90-B928-E996E1F53A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E99A6FF-C4F5-49C7-BBF3-848343A8D0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -1084,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,278 +1139,278 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B2">
-        <v>662.65521777397339</v>
+        <v>470.15663229742336</v>
       </c>
       <c r="C2">
-        <v>7934149622.8315115</v>
+        <v>8921474338.786293</v>
       </c>
       <c r="D2">
-        <v>11973269.673306623</v>
+        <v>18975536.504061323</v>
       </c>
       <c r="E2">
-        <v>0.60100490180918753</v>
+        <v>0.8836954720487562</v>
       </c>
       <c r="F2">
-        <v>125.59558798069767</v>
+        <v>133.16679170159205</v>
       </c>
       <c r="G2">
-        <v>453.6792383724395</v>
+        <v>319.46355316139619</v>
       </c>
       <c r="H2">
-        <v>-0.25256080837562622</v>
+        <v>-0.34650568426651729</v>
       </c>
       <c r="I2">
-        <v>-4.9472216575946248E-2</v>
+        <v>3.4409572293988999E-2</v>
       </c>
       <c r="J2">
-        <v>0.27171252735398754</v>
+        <v>0.58288993092918751</v>
       </c>
       <c r="K2">
-        <v>0.2512561872807817</v>
+        <v>0.46856790462369879</v>
       </c>
       <c r="L2">
-        <v>-8.2366239265637464E-2</v>
+        <v>-2.3420464129504381E-2</v>
       </c>
       <c r="M2">
-        <v>-0.24589697880793293</v>
+        <v>-0.35179038408891561</v>
       </c>
       <c r="N2">
-        <v>94.696214877447176</v>
+        <v>96.927408574309311</v>
       </c>
       <c r="O2">
-        <v>61.682595642255713</v>
+        <v>93.290786227371314</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B3">
-        <v>886.56739598288459</v>
+        <v>719.45022470427932</v>
       </c>
       <c r="C3">
-        <v>8347099118.1873665</v>
+        <v>8624702030.7452507</v>
       </c>
       <c r="D3">
-        <v>9415075.668255806</v>
+        <v>11987906.507764762</v>
       </c>
       <c r="E3">
-        <v>0.48032122271881494</v>
+        <v>0.60173960582040065</v>
       </c>
       <c r="F3">
-        <v>136.86897033974233</v>
+        <v>136.36041593160243</v>
       </c>
       <c r="G3">
-        <v>601.61440230709434</v>
+        <v>492.83988592544631</v>
       </c>
       <c r="H3">
-        <v>1.2158530364034017</v>
+        <v>-0.25294214079289401</v>
       </c>
       <c r="I3">
-        <v>-4.0858436680157206E-2</v>
+        <v>-4.9983832135574113E-2</v>
       </c>
       <c r="J3">
-        <v>-0.56714567818240957</v>
+        <v>0.27167682684274408</v>
       </c>
       <c r="K3">
-        <v>-0.50703672301460312</v>
+        <v>0.25122106103595776</v>
       </c>
       <c r="L3">
-        <v>8.6351440285316938E-2</v>
+        <v>-8.2189450562490274E-2</v>
       </c>
       <c r="M3">
-        <v>1.2216481187552026</v>
+        <v>-0.246553986261564</v>
       </c>
       <c r="N3">
-        <v>99.624878439982297</v>
+        <v>93.703124149707335</v>
       </c>
       <c r="O3">
-        <v>48.503568468100852</v>
+        <v>58.937001496122846</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B4">
-        <v>400.10207419797615</v>
+        <v>963.04485099436852</v>
       </c>
       <c r="C4">
-        <v>8702676890.8813076</v>
+        <v>9078479211.7096443</v>
       </c>
       <c r="D4">
-        <v>21751141.651355449</v>
+        <v>9426849.8526687324</v>
       </c>
       <c r="E4">
-        <v>0.97435497762857415</v>
+        <v>0.48092189666483548</v>
       </c>
       <c r="F4">
-        <v>125.98958795856649</v>
+        <v>148.57141924896419</v>
       </c>
       <c r="G4">
-        <v>270.79644036706452</v>
+        <v>654.11439829654353</v>
       </c>
       <c r="H4">
-        <v>-2.4701332369039264E-3</v>
+        <v>1.2134441067149506</v>
       </c>
       <c r="I4">
-        <v>1.4080583617405162E-2</v>
+        <v>-4.188692214530354E-2</v>
       </c>
       <c r="J4">
-        <v>1.6591700565332212E-2</v>
+        <v>-0.56713924921435421</v>
       </c>
       <c r="K4">
-        <v>1.0170212828736203E-2</v>
+        <v>-0.50702940127839669</v>
       </c>
       <c r="L4">
-        <v>6.3459591994674547E-3</v>
+        <v>8.47184440380222E-2</v>
       </c>
       <c r="M4">
-        <v>-1.8406972416513678E-3</v>
+        <v>1.2196723111014927</v>
       </c>
       <c r="N4">
-        <v>103.86879502453654</v>
+        <v>98.633188907032832</v>
       </c>
       <c r="O4">
-        <v>112.05517889813467</v>
+        <v>46.345895633286567</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B5">
-        <v>401.09282692083707</v>
+        <v>435.08885002913263</v>
       </c>
       <c r="C5">
-        <v>8581839581.0689087</v>
+        <v>9475373441.3449364</v>
       </c>
       <c r="D5">
-        <v>21396143.249309942</v>
+        <v>21778019.456739664</v>
       </c>
       <c r="E5">
-        <v>0.96454534617500731</v>
+        <v>0.97555898447490952</v>
       </c>
       <c r="F5">
-        <v>125.19510493070321</v>
+        <v>136.96772657048723</v>
       </c>
       <c r="G5">
-        <v>271.29581382324051</v>
+        <v>294.68962379043467</v>
       </c>
       <c r="H5">
-        <v>-3.6094428167074533E-2</v>
+        <v>-2.4139029120445743E-3</v>
       </c>
       <c r="I5">
-        <v>1.5247568031038439E-2</v>
+        <v>1.411651830421401E-2</v>
       </c>
       <c r="J5">
-        <v>5.3264549659654881E-2</v>
+        <v>1.6570420602805447E-2</v>
       </c>
       <c r="K5">
-        <v>4.9168678899710994E-2</v>
+        <v>1.0149067284991542E-2</v>
       </c>
       <c r="L5">
-        <v>-4.4919207430094144E-4</v>
+        <v>6.1435452387501588E-3</v>
       </c>
       <c r="M5">
-        <v>-3.0643239613244E-2</v>
+        <v>-1.673078925594762E-3</v>
       </c>
       <c r="N5">
-        <v>102.4265691529347</v>
+        <v>102.94524851688867</v>
       </c>
       <c r="O5">
-        <v>110.22633652804777</v>
+        <v>107.06883345086935</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B6">
-        <v>416.11215729164684</v>
+        <v>436.14165363691069</v>
       </c>
       <c r="C6">
-        <v>8452952611.0684977</v>
+        <v>9343476090.0941372</v>
       </c>
       <c r="D6">
-        <v>20314120.755534545</v>
+        <v>21423030.825376313</v>
       </c>
       <c r="E6">
-        <v>0.91934249046259153</v>
+        <v>0.96575744716267398</v>
       </c>
       <c r="F6">
-        <v>125.25136685198848</v>
+        <v>136.13139717353735</v>
       </c>
       <c r="G6">
-        <v>279.87199853539818</v>
+        <v>295.18348906517315</v>
       </c>
       <c r="H6">
-        <v>-3.5965088317736371E-2</v>
+        <v>-3.6186849785866837E-2</v>
       </c>
       <c r="I6">
-        <v>8.8826841671714174E-3</v>
+        <v>1.5122489958370178E-2</v>
       </c>
       <c r="J6">
-        <v>4.6520900790457453E-2</v>
+        <v>5.3235774727536489E-2</v>
       </c>
       <c r="K6">
-        <v>4.2159218877963145E-2</v>
+        <v>4.91400158657882E-2</v>
       </c>
       <c r="L6">
-        <v>1.1290411509541576E-2</v>
+        <v>-3.0022649526117995E-4</v>
       </c>
       <c r="M6">
-        <v>-3.9023886136794417E-2</v>
+        <v>-3.087473276982311E-2</v>
       </c>
       <c r="N6">
-        <v>100.88826841671714</v>
+        <v>101.51224899583701</v>
       </c>
       <c r="O6">
-        <v>104.65209007904575</v>
+        <v>105.32357747275366</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B7">
-        <v>431.63598356155103</v>
+        <v>452.51681152100053</v>
       </c>
       <c r="C7">
-        <v>8378528786.0762281</v>
+        <v>9204284391.8050823</v>
       </c>
       <c r="D7">
-        <v>19411098.947179075</v>
+        <v>20340204.291786686</v>
       </c>
       <c r="E7">
-        <v>0.88215166532077338</v>
+        <v>0.92052293550703623</v>
       </c>
       <c r="F7">
-        <v>123.85301534207885</v>
+        <v>136.17227969982335</v>
       </c>
       <c r="G7">
-        <v>291.23720610524748</v>
+        <v>304.58754822152844</v>
       </c>
       <c r="H7">
-        <v>-1.9200542076866833E-2</v>
+        <v>-3.5869632351568481E-2</v>
       </c>
       <c r="I7">
-        <v>6.5683161127729761E-3</v>
+        <v>8.9638823037501147E-3</v>
       </c>
       <c r="J7">
-        <v>2.6273320179240223E-2</v>
+        <v>4.6501506600886477E-2</v>
       </c>
       <c r="K7">
-        <v>1.8151797095498079E-2</v>
+        <v>4.2139905519349652E-2</v>
       </c>
       <c r="L7">
-        <v>1.6252900049103625E-2</v>
+        <v>1.1321105465380787E-2</v>
       </c>
       <c r="M7">
-        <v>-2.7344259646731262E-2</v>
+        <v>-3.8898520130888015E-2</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1428,7 +1428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated ace data file
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E99A6FF-C4F5-49C7-BBF3-848343A8D0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCFD60D-2778-405A-BFD8-99B52B8A9CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,13 +192,13 @@
     <t>SMATSA</t>
   </si>
   <si>
-    <t>UkSATSE</t>
-  </si>
-  <si>
     <t>BHANSA</t>
   </si>
   <si>
     <t>HASP</t>
+  </si>
+  <si>
+    <t>HCAA</t>
   </si>
 </sst>
 </file>
@@ -786,9 +786,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -826,7 +826,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -932,7 +932,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1074,7 +1074,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1085,7 +1085,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:O7"/>
+      <selection sqref="A1:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,46 +1142,46 @@
         <v>2022</v>
       </c>
       <c r="B2">
-        <v>470.15663229742336</v>
+        <v>470.26551030000002</v>
       </c>
       <c r="C2">
-        <v>8921474338.786293</v>
+        <v>8923563036</v>
       </c>
       <c r="D2">
-        <v>18975536.504061323</v>
+        <v>18975584.73</v>
       </c>
       <c r="E2">
-        <v>0.8836954720487562</v>
+        <v>0.88557406599999999</v>
       </c>
       <c r="F2">
-        <v>133.16679170159205</v>
+        <v>133.29054529999999</v>
       </c>
       <c r="G2">
-        <v>319.46355316139619</v>
+        <v>319.75235679999997</v>
       </c>
       <c r="H2">
-        <v>-0.34650568426651729</v>
+        <v>-0.34658558099999998</v>
       </c>
       <c r="I2">
-        <v>3.4409572293988999E-2</v>
+        <v>3.4281998000000001E-2</v>
       </c>
       <c r="J2">
-        <v>0.58288993092918751</v>
+        <v>0.58288823599999995</v>
       </c>
       <c r="K2">
-        <v>0.46856790462369879</v>
+        <v>0.46956072599999998</v>
       </c>
       <c r="L2">
-        <v>-2.3420464129504381E-2</v>
+        <v>-2.3923535999999999E-2</v>
       </c>
       <c r="M2">
-        <v>-0.35179038408891561</v>
+        <v>-0.35154045499999997</v>
       </c>
       <c r="N2">
-        <v>96.927408574309311</v>
+        <v>96.950101239999995</v>
       </c>
       <c r="O2">
-        <v>93.290786227371314</v>
+        <v>93.290669390000005</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1189,46 +1189,46 @@
         <v>2021</v>
       </c>
       <c r="B3">
-        <v>719.45022470427932</v>
+        <v>719.70482509999999</v>
       </c>
       <c r="C3">
-        <v>8624702030.7452507</v>
+        <v>8627785321</v>
       </c>
       <c r="D3">
-        <v>11987906.507764762</v>
+        <v>11987949.810000001</v>
       </c>
       <c r="E3">
-        <v>0.60173960582040065</v>
+        <v>0.60261141299999998</v>
       </c>
       <c r="F3">
-        <v>136.36041593160243</v>
+        <v>136.55748320000001</v>
       </c>
       <c r="G3">
-        <v>492.83988592544631</v>
+        <v>493.09530489999997</v>
       </c>
       <c r="H3">
-        <v>-0.25294214079289401</v>
+        <v>-0.25295200800000001</v>
       </c>
       <c r="I3">
-        <v>-4.9983832135574113E-2</v>
+        <v>-4.9996459E-2</v>
       </c>
       <c r="J3">
-        <v>0.27167682684274408</v>
+        <v>0.27167672100000001</v>
       </c>
       <c r="K3">
-        <v>0.25122106103595776</v>
+        <v>0.25134547499999998</v>
       </c>
       <c r="L3">
-        <v>-8.2189450562490274E-2</v>
+        <v>-8.2098113E-2</v>
       </c>
       <c r="M3">
-        <v>-0.246553986261564</v>
+        <v>-0.246572025</v>
       </c>
       <c r="N3">
-        <v>93.703124149707335</v>
+        <v>93.736622569999994</v>
       </c>
       <c r="O3">
-        <v>58.937001496122846</v>
+        <v>58.936990790000003</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1236,46 +1236,46 @@
         <v>2020</v>
       </c>
       <c r="B4">
-        <v>963.04485099436852</v>
+        <v>963.39837990000001</v>
       </c>
       <c r="C4">
-        <v>9078479211.7096443</v>
+        <v>9081845434</v>
       </c>
       <c r="D4">
-        <v>9426849.8526687324</v>
+        <v>9426884.6850000005</v>
       </c>
       <c r="E4">
-        <v>0.48092189666483548</v>
+        <v>0.48157077700000001</v>
       </c>
       <c r="F4">
-        <v>148.57141924896419</v>
+        <v>148.77132850000001</v>
       </c>
       <c r="G4">
-        <v>654.11439829654353</v>
+        <v>654.46906869999998</v>
       </c>
       <c r="H4">
-        <v>1.2134441067149506</v>
+        <v>1.213430842</v>
       </c>
       <c r="I4">
-        <v>-4.188692214530354E-2</v>
+        <v>-4.1892621999999997E-2</v>
       </c>
       <c r="J4">
-        <v>-0.56713924921435421</v>
+        <v>-0.56713922999999999</v>
       </c>
       <c r="K4">
-        <v>-0.50702940127839669</v>
+        <v>-0.50710518000000004</v>
       </c>
       <c r="L4">
-        <v>8.47184440380222E-2</v>
+        <v>8.4551656000000003E-2</v>
       </c>
       <c r="M4">
-        <v>1.2196723111014927</v>
+        <v>1.219649314</v>
       </c>
       <c r="N4">
-        <v>98.633188907032832</v>
+        <v>98.669761249999993</v>
       </c>
       <c r="O4">
-        <v>46.345895633286567</v>
+        <v>46.34589106</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1283,46 +1283,46 @@
         <v>2019</v>
       </c>
       <c r="B5">
-        <v>435.08885002913263</v>
+        <v>435.25117729999999</v>
       </c>
       <c r="C5">
-        <v>9475373441.3449364</v>
+        <v>9478943216</v>
       </c>
       <c r="D5">
-        <v>21778019.456739664</v>
+        <v>21778098.969999999</v>
       </c>
       <c r="E5">
-        <v>0.97555898447490952</v>
+        <v>0.977025437</v>
       </c>
       <c r="F5">
-        <v>136.96772657048723</v>
+        <v>137.1731145</v>
       </c>
       <c r="G5">
-        <v>294.68962379043467</v>
+        <v>294.85246369999999</v>
       </c>
       <c r="H5">
-        <v>-2.4139029120445743E-3</v>
+        <v>-2.038008E-3</v>
       </c>
       <c r="I5">
-        <v>1.411651830421401E-2</v>
+        <v>1.4498578999999999E-2</v>
       </c>
       <c r="J5">
-        <v>1.6570420602805447E-2</v>
+        <v>1.6570358E-2</v>
       </c>
       <c r="K5">
-        <v>1.0149067284991542E-2</v>
+        <v>1.0387739E-2</v>
       </c>
       <c r="L5">
-        <v>6.1435452387501588E-3</v>
+        <v>6.3813330000000003E-3</v>
       </c>
       <c r="M5">
-        <v>-1.673078925594762E-3</v>
+        <v>-1.1177139999999999E-3</v>
       </c>
       <c r="N5">
-        <v>102.94524851688867</v>
+        <v>102.9840324</v>
       </c>
       <c r="O5">
-        <v>107.06883345086935</v>
+        <v>107.0688182</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1330,46 +1330,46 @@
         <v>2018</v>
       </c>
       <c r="B6">
-        <v>436.14165363691069</v>
+        <v>436.1400342</v>
       </c>
       <c r="C6">
-        <v>9343476090.0941372</v>
+        <v>9343476090</v>
       </c>
       <c r="D6">
-        <v>21423030.825376313</v>
+        <v>21423110.370000001</v>
       </c>
       <c r="E6">
-        <v>0.96575744716267398</v>
+        <v>0.96698069399999997</v>
       </c>
       <c r="F6">
-        <v>136.13139717353735</v>
+        <v>136.30331770000001</v>
       </c>
       <c r="G6">
-        <v>295.18348906517315</v>
+        <v>295.18239299999999</v>
       </c>
       <c r="H6">
-        <v>-3.6186849785866837E-2</v>
+        <v>-3.6186771999999999E-2</v>
       </c>
       <c r="I6">
-        <v>1.5122489958370178E-2</v>
+        <v>1.5122490000000001E-2</v>
       </c>
       <c r="J6">
-        <v>5.3235774727536489E-2</v>
+        <v>5.3235690000000002E-2</v>
       </c>
       <c r="K6">
-        <v>4.91400158657882E-2</v>
+        <v>4.9273702000000003E-2</v>
       </c>
       <c r="L6">
-        <v>-3.0022649526117995E-4</v>
+        <v>-1.7275999999999999E-4</v>
       </c>
       <c r="M6">
-        <v>-3.087473276982311E-2</v>
+        <v>-3.0874655000000001E-2</v>
       </c>
       <c r="N6">
-        <v>101.51224899583701</v>
+        <v>101.512249</v>
       </c>
       <c r="O6">
-        <v>105.32357747275366</v>
+        <v>105.32356900000001</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1377,40 +1377,40 @@
         <v>2017</v>
       </c>
       <c r="B7">
-        <v>452.51681152100053</v>
+        <v>452.51509479999999</v>
       </c>
       <c r="C7">
-        <v>9204284391.8050823</v>
+        <v>9204284392</v>
       </c>
       <c r="D7">
-        <v>20340204.291786686</v>
+        <v>20340281.460000001</v>
       </c>
       <c r="E7">
-        <v>0.92052293550703623</v>
+        <v>0.92157145699999998</v>
       </c>
       <c r="F7">
-        <v>136.17227969982335</v>
+        <v>136.32686949999999</v>
       </c>
       <c r="G7">
-        <v>304.58754822152844</v>
+        <v>304.58639269999998</v>
       </c>
       <c r="H7">
-        <v>-3.5869632351568481E-2</v>
+        <v>-3.5869579999999998E-2</v>
       </c>
       <c r="I7">
-        <v>8.9638823037501147E-3</v>
+        <v>8.9638819999999994E-3</v>
       </c>
       <c r="J7">
-        <v>4.6501506600886477E-2</v>
+        <v>4.6501449E-2</v>
       </c>
       <c r="K7">
-        <v>4.2139905519349652E-2</v>
+        <v>4.3322938999999998E-2</v>
       </c>
       <c r="L7">
-        <v>1.1321105465380787E-2</v>
+        <v>1.2469209E-2</v>
       </c>
       <c r="M7">
-        <v>-3.8898520130888015E-2</v>
+        <v>-3.8898467999999999E-2</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1429,7 +1429,7 @@
   <dimension ref="A1:A40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A2" sqref="A2:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1524,117 +1524,117 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated list of ANSPs for ACE
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCFD60D-2778-405A-BFD8-99B52B8A9CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6412CF9-0335-4BB7-8D51-C2F4D47FF6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>year_data</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>HASP</t>
-  </si>
-  <si>
-    <t>HCAA</t>
   </si>
 </sst>
 </file>
@@ -528,7 +525,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -663,17 +660,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF999999"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -719,14 +705,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1084,7 +1069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:O7"/>
     </sheetView>
   </sheetViews>
@@ -1426,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,111 +1514,106 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
202406 June full release
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E99A6FF-C4F5-49C7-BBF3-848343A8D0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6412CF9-0335-4BB7-8D51-C2F4D47FF6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>year_data</t>
   </si>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>SMATSA</t>
-  </si>
-  <si>
-    <t>UkSATSE</t>
   </si>
   <si>
     <t>BHANSA</t>
@@ -528,7 +525,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -663,17 +660,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF999999"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -719,14 +705,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -786,9 +771,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -826,7 +811,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -932,7 +917,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1074,7 +1059,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1084,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:O7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,46 +1127,46 @@
         <v>2022</v>
       </c>
       <c r="B2">
-        <v>470.15663229742336</v>
+        <v>470.26551030000002</v>
       </c>
       <c r="C2">
-        <v>8921474338.786293</v>
+        <v>8923563036</v>
       </c>
       <c r="D2">
-        <v>18975536.504061323</v>
+        <v>18975584.73</v>
       </c>
       <c r="E2">
-        <v>0.8836954720487562</v>
+        <v>0.88557406599999999</v>
       </c>
       <c r="F2">
-        <v>133.16679170159205</v>
+        <v>133.29054529999999</v>
       </c>
       <c r="G2">
-        <v>319.46355316139619</v>
+        <v>319.75235679999997</v>
       </c>
       <c r="H2">
-        <v>-0.34650568426651729</v>
+        <v>-0.34658558099999998</v>
       </c>
       <c r="I2">
-        <v>3.4409572293988999E-2</v>
+        <v>3.4281998000000001E-2</v>
       </c>
       <c r="J2">
-        <v>0.58288993092918751</v>
+        <v>0.58288823599999995</v>
       </c>
       <c r="K2">
-        <v>0.46856790462369879</v>
+        <v>0.46956072599999998</v>
       </c>
       <c r="L2">
-        <v>-2.3420464129504381E-2</v>
+        <v>-2.3923535999999999E-2</v>
       </c>
       <c r="M2">
-        <v>-0.35179038408891561</v>
+        <v>-0.35154045499999997</v>
       </c>
       <c r="N2">
-        <v>96.927408574309311</v>
+        <v>96.950101239999995</v>
       </c>
       <c r="O2">
-        <v>93.290786227371314</v>
+        <v>93.290669390000005</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1189,46 +1174,46 @@
         <v>2021</v>
       </c>
       <c r="B3">
-        <v>719.45022470427932</v>
+        <v>719.70482509999999</v>
       </c>
       <c r="C3">
-        <v>8624702030.7452507</v>
+        <v>8627785321</v>
       </c>
       <c r="D3">
-        <v>11987906.507764762</v>
+        <v>11987949.810000001</v>
       </c>
       <c r="E3">
-        <v>0.60173960582040065</v>
+        <v>0.60261141299999998</v>
       </c>
       <c r="F3">
-        <v>136.36041593160243</v>
+        <v>136.55748320000001</v>
       </c>
       <c r="G3">
-        <v>492.83988592544631</v>
+        <v>493.09530489999997</v>
       </c>
       <c r="H3">
-        <v>-0.25294214079289401</v>
+        <v>-0.25295200800000001</v>
       </c>
       <c r="I3">
-        <v>-4.9983832135574113E-2</v>
+        <v>-4.9996459E-2</v>
       </c>
       <c r="J3">
-        <v>0.27167682684274408</v>
+        <v>0.27167672100000001</v>
       </c>
       <c r="K3">
-        <v>0.25122106103595776</v>
+        <v>0.25134547499999998</v>
       </c>
       <c r="L3">
-        <v>-8.2189450562490274E-2</v>
+        <v>-8.2098113E-2</v>
       </c>
       <c r="M3">
-        <v>-0.246553986261564</v>
+        <v>-0.246572025</v>
       </c>
       <c r="N3">
-        <v>93.703124149707335</v>
+        <v>93.736622569999994</v>
       </c>
       <c r="O3">
-        <v>58.937001496122846</v>
+        <v>58.936990790000003</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1236,46 +1221,46 @@
         <v>2020</v>
       </c>
       <c r="B4">
-        <v>963.04485099436852</v>
+        <v>963.39837990000001</v>
       </c>
       <c r="C4">
-        <v>9078479211.7096443</v>
+        <v>9081845434</v>
       </c>
       <c r="D4">
-        <v>9426849.8526687324</v>
+        <v>9426884.6850000005</v>
       </c>
       <c r="E4">
-        <v>0.48092189666483548</v>
+        <v>0.48157077700000001</v>
       </c>
       <c r="F4">
-        <v>148.57141924896419</v>
+        <v>148.77132850000001</v>
       </c>
       <c r="G4">
-        <v>654.11439829654353</v>
+        <v>654.46906869999998</v>
       </c>
       <c r="H4">
-        <v>1.2134441067149506</v>
+        <v>1.213430842</v>
       </c>
       <c r="I4">
-        <v>-4.188692214530354E-2</v>
+        <v>-4.1892621999999997E-2</v>
       </c>
       <c r="J4">
-        <v>-0.56713924921435421</v>
+        <v>-0.56713922999999999</v>
       </c>
       <c r="K4">
-        <v>-0.50702940127839669</v>
+        <v>-0.50710518000000004</v>
       </c>
       <c r="L4">
-        <v>8.47184440380222E-2</v>
+        <v>8.4551656000000003E-2</v>
       </c>
       <c r="M4">
-        <v>1.2196723111014927</v>
+        <v>1.219649314</v>
       </c>
       <c r="N4">
-        <v>98.633188907032832</v>
+        <v>98.669761249999993</v>
       </c>
       <c r="O4">
-        <v>46.345895633286567</v>
+        <v>46.34589106</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1283,46 +1268,46 @@
         <v>2019</v>
       </c>
       <c r="B5">
-        <v>435.08885002913263</v>
+        <v>435.25117729999999</v>
       </c>
       <c r="C5">
-        <v>9475373441.3449364</v>
+        <v>9478943216</v>
       </c>
       <c r="D5">
-        <v>21778019.456739664</v>
+        <v>21778098.969999999</v>
       </c>
       <c r="E5">
-        <v>0.97555898447490952</v>
+        <v>0.977025437</v>
       </c>
       <c r="F5">
-        <v>136.96772657048723</v>
+        <v>137.1731145</v>
       </c>
       <c r="G5">
-        <v>294.68962379043467</v>
+        <v>294.85246369999999</v>
       </c>
       <c r="H5">
-        <v>-2.4139029120445743E-3</v>
+        <v>-2.038008E-3</v>
       </c>
       <c r="I5">
-        <v>1.411651830421401E-2</v>
+        <v>1.4498578999999999E-2</v>
       </c>
       <c r="J5">
-        <v>1.6570420602805447E-2</v>
+        <v>1.6570358E-2</v>
       </c>
       <c r="K5">
-        <v>1.0149067284991542E-2</v>
+        <v>1.0387739E-2</v>
       </c>
       <c r="L5">
-        <v>6.1435452387501588E-3</v>
+        <v>6.3813330000000003E-3</v>
       </c>
       <c r="M5">
-        <v>-1.673078925594762E-3</v>
+        <v>-1.1177139999999999E-3</v>
       </c>
       <c r="N5">
-        <v>102.94524851688867</v>
+        <v>102.9840324</v>
       </c>
       <c r="O5">
-        <v>107.06883345086935</v>
+        <v>107.0688182</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1330,46 +1315,46 @@
         <v>2018</v>
       </c>
       <c r="B6">
-        <v>436.14165363691069</v>
+        <v>436.1400342</v>
       </c>
       <c r="C6">
-        <v>9343476090.0941372</v>
+        <v>9343476090</v>
       </c>
       <c r="D6">
-        <v>21423030.825376313</v>
+        <v>21423110.370000001</v>
       </c>
       <c r="E6">
-        <v>0.96575744716267398</v>
+        <v>0.96698069399999997</v>
       </c>
       <c r="F6">
-        <v>136.13139717353735</v>
+        <v>136.30331770000001</v>
       </c>
       <c r="G6">
-        <v>295.18348906517315</v>
+        <v>295.18239299999999</v>
       </c>
       <c r="H6">
-        <v>-3.6186849785866837E-2</v>
+        <v>-3.6186771999999999E-2</v>
       </c>
       <c r="I6">
-        <v>1.5122489958370178E-2</v>
+        <v>1.5122490000000001E-2</v>
       </c>
       <c r="J6">
-        <v>5.3235774727536489E-2</v>
+        <v>5.3235690000000002E-2</v>
       </c>
       <c r="K6">
-        <v>4.91400158657882E-2</v>
+        <v>4.9273702000000003E-2</v>
       </c>
       <c r="L6">
-        <v>-3.0022649526117995E-4</v>
+        <v>-1.7275999999999999E-4</v>
       </c>
       <c r="M6">
-        <v>-3.087473276982311E-2</v>
+        <v>-3.0874655000000001E-2</v>
       </c>
       <c r="N6">
-        <v>101.51224899583701</v>
+        <v>101.512249</v>
       </c>
       <c r="O6">
-        <v>105.32357747275366</v>
+        <v>105.32356900000001</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1377,40 +1362,40 @@
         <v>2017</v>
       </c>
       <c r="B7">
-        <v>452.51681152100053</v>
+        <v>452.51509479999999</v>
       </c>
       <c r="C7">
-        <v>9204284391.8050823</v>
+        <v>9204284392</v>
       </c>
       <c r="D7">
-        <v>20340204.291786686</v>
+        <v>20340281.460000001</v>
       </c>
       <c r="E7">
-        <v>0.92052293550703623</v>
+        <v>0.92157145699999998</v>
       </c>
       <c r="F7">
-        <v>136.17227969982335</v>
+        <v>136.32686949999999</v>
       </c>
       <c r="G7">
-        <v>304.58754822152844</v>
+        <v>304.58639269999998</v>
       </c>
       <c r="H7">
-        <v>-3.5869632351568481E-2</v>
+        <v>-3.5869579999999998E-2</v>
       </c>
       <c r="I7">
-        <v>8.9638823037501147E-3</v>
+        <v>8.9638819999999994E-3</v>
       </c>
       <c r="J7">
-        <v>4.6501506600886477E-2</v>
+        <v>4.6501449E-2</v>
       </c>
       <c r="K7">
-        <v>4.2139905519349652E-2</v>
+        <v>4.3322938999999998E-2</v>
       </c>
       <c r="L7">
-        <v>1.1321105465380787E-2</v>
+        <v>1.2469209E-2</v>
       </c>
       <c r="M7">
-        <v>-3.8898520130888015E-2</v>
+        <v>-3.8898467999999999E-2</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1426,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,7 +1454,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1524,7 +1509,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -1630,11 +1615,6 @@
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed IAA by Airnav Ireland for ACE factsheets list
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6412CF9-0335-4BB7-8D51-C2F4D47FF6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BB22FD-F332-496C-B80E-FDCDA4CB0993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>HungaroControl</t>
   </si>
   <si>
-    <t>IAA</t>
-  </si>
-  <si>
     <t>LFV</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>HASP</t>
+  </si>
+  <si>
+    <t>AirNav Ireland</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1414,7 @@
   <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1509,7 +1509,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -1519,102 +1519,102 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
202407 July full release
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6412CF9-0335-4BB7-8D51-C2F4D47FF6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BB22FD-F332-496C-B80E-FDCDA4CB0993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>HungaroControl</t>
   </si>
   <si>
-    <t>IAA</t>
-  </si>
-  <si>
     <t>LFV</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>HASP</t>
+  </si>
+  <si>
+    <t>AirNav Ireland</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1414,7 @@
   <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1509,7 +1509,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -1519,102 +1519,102 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added hlsr 2023 to ace landing page
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BB22FD-F332-496C-B80E-FDCDA4CB0993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBD7117-9B27-438E-BEA7-8DACAA4AE6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>year_data</t>
   </si>
@@ -195,7 +195,10 @@
     <t>HASP</t>
   </si>
   <si>
-    <t>AirNav Ireland</t>
+    <t>Airnav Ireland</t>
+  </si>
+  <si>
+    <t>IAA</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1073,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:O7"/>
+      <selection activeCell="A2" sqref="A2:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,278 +1127,278 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B2">
-        <v>470.26551030000002</v>
+        <v>459.75478594995815</v>
       </c>
       <c r="C2">
-        <v>8923563036</v>
+        <v>9697453988.650034</v>
       </c>
       <c r="D2">
-        <v>18975584.73</v>
+        <v>21092665.666574594</v>
       </c>
       <c r="E2">
-        <v>0.88557406599999999</v>
+        <v>0.96487719841975128</v>
       </c>
       <c r="F2">
-        <v>133.29054529999999</v>
+        <v>143.23688519223813</v>
       </c>
       <c r="G2">
-        <v>319.75235679999997</v>
+        <v>311.30388937283158</v>
       </c>
       <c r="H2">
-        <v>-0.34658558099999998</v>
+        <v>-7.3401833037353037E-2</v>
       </c>
       <c r="I2">
-        <v>3.4281998000000001E-2</v>
+        <v>2.881493514775868E-2</v>
       </c>
       <c r="J2">
-        <v>0.58288823599999995</v>
+        <v>0.1103140194202783</v>
       </c>
       <c r="K2">
-        <v>0.46956072599999998</v>
+        <v>8.7627141137734288E-2</v>
       </c>
       <c r="L2">
-        <v>-2.3923535999999999E-2</v>
+        <v>1.9373872608318132E-2</v>
       </c>
       <c r="M2">
-        <v>-0.35154045499999997</v>
+        <v>-7.8394576610962274E-2</v>
       </c>
       <c r="N2">
-        <v>96.950101239999995</v>
+        <v>98.083295763940995</v>
       </c>
       <c r="O2">
-        <v>93.290669390000005</v>
+        <v>98.340013892985766</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B3">
-        <v>719.70482509999999</v>
+        <v>496.17493574050184</v>
       </c>
       <c r="C3">
-        <v>8627785321</v>
+        <v>9425848767.6962852</v>
       </c>
       <c r="D3">
-        <v>11987949.810000001</v>
+        <v>18997027.235220883</v>
       </c>
       <c r="E3">
-        <v>0.60261141299999998</v>
+        <v>0.88713968411124977</v>
       </c>
       <c r="F3">
-        <v>136.55748320000001</v>
+        <v>140.5145737409685</v>
       </c>
       <c r="G3">
-        <v>493.09530489999997</v>
+        <v>337.78435051745646</v>
       </c>
       <c r="H3">
-        <v>-0.25295200800000001</v>
+        <v>-0.3463303356472609</v>
       </c>
       <c r="I3">
-        <v>-4.9996459E-2</v>
+        <v>3.4652402249871983E-2</v>
       </c>
       <c r="J3">
-        <v>0.27167672100000001</v>
+        <v>0.58283680377669089</v>
       </c>
       <c r="K3">
-        <v>0.25134547499999998</v>
+        <v>0.46942846730010523</v>
       </c>
       <c r="L3">
-        <v>-8.2098113E-2</v>
+        <v>-2.2739401580627816E-2</v>
       </c>
       <c r="M3">
-        <v>-0.246572025</v>
+        <v>-0.35153884325092255</v>
       </c>
       <c r="N3">
-        <v>93.736622569999994</v>
+        <v>95.336189642167525</v>
       </c>
       <c r="O3">
-        <v>58.936990790000003</v>
+        <v>88.569550751355436</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B4">
-        <v>963.39837990000001</v>
+        <v>759.06067360768861</v>
       </c>
       <c r="C4">
-        <v>9081845434</v>
+        <v>9110159844.213953</v>
       </c>
       <c r="D4">
-        <v>9426884.6850000005</v>
+        <v>12001886.227243055</v>
       </c>
       <c r="E4">
-        <v>0.48157077700000001</v>
+        <v>0.60373111305054561</v>
       </c>
       <c r="F4">
-        <v>148.77132850000001</v>
+        <v>143.78413901904744</v>
       </c>
       <c r="G4">
-        <v>654.46906869999998</v>
+        <v>520.90144028189241</v>
       </c>
       <c r="H4">
-        <v>1.213430842</v>
+        <v>-0.25298124827727519</v>
       </c>
       <c r="I4">
-        <v>-4.1892621999999997E-2</v>
+        <v>-5.0058973750314206E-2</v>
       </c>
       <c r="J4">
-        <v>-0.56713922999999999</v>
+        <v>0.27164281225738329</v>
       </c>
       <c r="K4">
-        <v>-0.50710518000000004</v>
+        <v>0.25218144054202773</v>
       </c>
       <c r="L4">
-        <v>8.4551656000000003E-2</v>
+        <v>-8.2298725560155828E-2</v>
       </c>
       <c r="M4">
-        <v>1.219649314</v>
+        <v>-0.24633456259909303</v>
       </c>
       <c r="N4">
-        <v>98.669761249999993</v>
+        <v>92.143206196455068</v>
       </c>
       <c r="O4">
-        <v>46.34589106</v>
+        <v>55.956211366848507</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B5">
-        <v>435.25117729999999</v>
+        <v>1016.1199727010782</v>
       </c>
       <c r="C5">
-        <v>9478943216</v>
+        <v>9590237280.4976711</v>
       </c>
       <c r="D5">
-        <v>21778098.969999999</v>
+        <v>9438095.4396601785</v>
       </c>
       <c r="E5">
-        <v>0.977025437</v>
+        <v>0.4821434765789297</v>
       </c>
       <c r="F5">
-        <v>137.1731145</v>
+        <v>156.67858705635106</v>
       </c>
       <c r="G5">
-        <v>294.85246369999999</v>
+        <v>691.15739482266133</v>
       </c>
       <c r="H5">
-        <v>-2.038008E-3</v>
+        <v>1.2101261251179785</v>
       </c>
       <c r="I5">
-        <v>1.4498578999999999E-2</v>
+        <v>-4.3309607927320526E-2</v>
       </c>
       <c r="J5">
-        <v>1.6570358E-2</v>
+        <v>-0.56713312367111612</v>
       </c>
       <c r="K5">
-        <v>1.0387739E-2</v>
+        <v>-0.50709822624514778</v>
       </c>
       <c r="L5">
-        <v>6.3813330000000003E-3</v>
+        <v>8.3028081427743317E-2</v>
       </c>
       <c r="M5">
-        <v>-1.1177139999999999E-3</v>
+        <v>1.2162327457674529</v>
       </c>
       <c r="N5">
-        <v>102.9840324</v>
+        <v>96.998870088000416</v>
       </c>
       <c r="O5">
-        <v>107.0688182</v>
+        <v>44.003088624797613</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B6">
-        <v>436.1400342</v>
+        <v>459.75655468388112</v>
       </c>
       <c r="C6">
-        <v>9343476090</v>
+        <v>10024389666.671915</v>
       </c>
       <c r="D6">
-        <v>21423110.370000001</v>
+        <v>21803690.593523942</v>
       </c>
       <c r="E6">
-        <v>0.96698069399999997</v>
+        <v>0.97817354745151885</v>
       </c>
       <c r="F6">
-        <v>136.30331770000001</v>
+        <v>144.66715105835806</v>
       </c>
       <c r="G6">
-        <v>295.18239299999999</v>
+        <v>311.86137653756327</v>
       </c>
       <c r="H6">
-        <v>-3.6186771999999999E-2</v>
+        <v>-2.6066784032476864E-3</v>
       </c>
       <c r="I6">
-        <v>1.5122490000000001E-2</v>
+        <v>1.3900326498015536E-2</v>
       </c>
       <c r="J6">
-        <v>5.3235690000000002E-2</v>
+        <v>1.6550145808913896E-2</v>
       </c>
       <c r="K6">
-        <v>4.9273702000000003E-2</v>
+        <v>1.0367650232698367E-2</v>
       </c>
       <c r="L6">
-        <v>-1.7275999999999999E-4</v>
+        <v>5.753828532776728E-3</v>
       </c>
       <c r="M6">
-        <v>-3.0874655000000001E-2</v>
+        <v>-1.6745752680884518E-3</v>
       </c>
       <c r="N6">
-        <v>101.512249</v>
+        <v>101.39003264980155</v>
       </c>
       <c r="O6">
-        <v>105.32356900000001</v>
+        <v>101.65501458089139</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B7">
-        <v>452.51509479999999</v>
+        <v>460.95812427122047</v>
       </c>
       <c r="C7">
-        <v>9204284392</v>
+        <v>9886957726.2055798</v>
       </c>
       <c r="D7">
-        <v>20340281.460000001</v>
+        <v>21448711.29419177</v>
       </c>
       <c r="E7">
-        <v>0.92157145699999998</v>
+        <v>0.9681362494397312</v>
       </c>
       <c r="F7">
-        <v>136.32686949999999</v>
+        <v>143.8395231061688</v>
       </c>
       <c r="G7">
-        <v>304.58639269999998</v>
+        <v>312.38448787509338</v>
       </c>
       <c r="H7">
-        <v>-3.5869579999999998E-2</v>
+        <v>-3.5645247613669828E-2</v>
       </c>
       <c r="I7">
-        <v>8.9638819999999994E-3</v>
+        <v>1.566648765768841E-2</v>
       </c>
       <c r="J7">
-        <v>4.6501449E-2</v>
+        <v>5.3208360454890302E-2</v>
       </c>
       <c r="K7">
-        <v>4.3322938999999998E-2</v>
+        <v>4.924647508858393E-2</v>
       </c>
       <c r="L7">
-        <v>1.2469209E-2</v>
+        <v>4.1615133750116939E-6</v>
       </c>
       <c r="M7">
-        <v>-3.8898467999999999E-2</v>
+        <v>-3.0183232751069267E-2</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1411,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,191 +1432,196 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ace data file corrected and data refreshed
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBD7117-9B27-438E-BEA7-8DACAA4AE6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A847A67F-A04D-4027-AB32-A1C8D18B20F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,7 +528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -663,6 +663,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -708,13 +719,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1130,46 +1142,46 @@
         <v>2023</v>
       </c>
       <c r="B2">
-        <v>459.75478594995815</v>
+        <v>459.75620180305265</v>
       </c>
       <c r="C2">
-        <v>9697453988.650034</v>
+        <v>9697483659.9791355</v>
       </c>
       <c r="D2">
-        <v>21092665.666574594</v>
+        <v>21092665.247250497</v>
       </c>
       <c r="E2">
-        <v>0.96487719841975128</v>
+        <v>0.96697865414991746</v>
       </c>
       <c r="F2">
-        <v>143.23688519223813</v>
+        <v>143.54928009986031</v>
       </c>
       <c r="G2">
-        <v>311.30388937283158</v>
+        <v>311.30485855591945</v>
       </c>
       <c r="H2">
-        <v>-7.3401833037353037E-2</v>
+        <v>-7.340211528671825E-2</v>
       </c>
       <c r="I2">
-        <v>2.881493514775868E-2</v>
+        <v>2.8814621788030959E-2</v>
       </c>
       <c r="J2">
-        <v>0.1103140194202783</v>
+        <v>0.11031401944801345</v>
       </c>
       <c r="K2">
-        <v>8.7627141137734288E-2</v>
+        <v>8.9995961984757455E-2</v>
       </c>
       <c r="L2">
-        <v>1.9373872608318132E-2</v>
+        <v>2.1593707224610625E-2</v>
       </c>
       <c r="M2">
-        <v>-7.8394576610962274E-2</v>
+        <v>-7.8394847778735288E-2</v>
       </c>
       <c r="N2">
-        <v>98.083295763940995</v>
+        <v>98.083315010808363</v>
       </c>
       <c r="O2">
-        <v>98.340013892985766</v>
+        <v>98.3400140079209</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1177,46 +1189,46 @@
         <v>2022</v>
       </c>
       <c r="B3">
-        <v>496.17493574050184</v>
+        <v>496.17661489192318</v>
       </c>
       <c r="C3">
-        <v>9425848767.6962852</v>
+        <v>9425880478.9587555</v>
       </c>
       <c r="D3">
-        <v>18997027.235220883</v>
+        <v>18997026.85708373</v>
       </c>
       <c r="E3">
-        <v>0.88713968411124977</v>
+        <v>0.88713966645267239</v>
       </c>
       <c r="F3">
-        <v>140.5145737409685</v>
+        <v>140.51503947674487</v>
       </c>
       <c r="G3">
-        <v>337.78435051745646</v>
+        <v>337.7855015302469</v>
       </c>
       <c r="H3">
-        <v>-0.3463303356472609</v>
+        <v>-0.34632988644957596</v>
       </c>
       <c r="I3">
-        <v>3.4652402249871983E-2</v>
+        <v>3.4653113848693406E-2</v>
       </c>
       <c r="J3">
-        <v>0.58283680377669089</v>
+        <v>0.58283680468264287</v>
       </c>
       <c r="K3">
-        <v>0.46942846730010523</v>
+        <v>0.46942846814114647</v>
       </c>
       <c r="L3">
-        <v>-2.2739401580627816E-2</v>
+        <v>-2.2738787926019133E-2</v>
       </c>
       <c r="M3">
-        <v>-0.35153884325092255</v>
+        <v>-0.35153837951542866</v>
       </c>
       <c r="N3">
-        <v>95.336189642167525</v>
+        <v>95.336237387785403</v>
       </c>
       <c r="O3">
-        <v>88.569550751355436</v>
+        <v>88.569550852658878</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1224,46 +1236,46 @@
         <v>2021</v>
       </c>
       <c r="B4">
-        <v>759.06067360768861</v>
+        <v>759.06272079188182</v>
       </c>
       <c r="C4">
-        <v>9110159844.213953</v>
+        <v>9110184227.7325668</v>
       </c>
       <c r="D4">
-        <v>12001886.227243055</v>
+        <v>12001885.981475275</v>
       </c>
       <c r="E4">
-        <v>0.60373111305054561</v>
+        <v>0.60373110068768443</v>
       </c>
       <c r="F4">
-        <v>143.78413901904744</v>
+        <v>143.78452530469158</v>
       </c>
       <c r="G4">
-        <v>520.90144028189241</v>
+        <v>520.90284275857732</v>
       </c>
       <c r="H4">
-        <v>-0.25298124827727519</v>
+        <v>-0.25298131630137988</v>
       </c>
       <c r="I4">
-        <v>-5.0058973750314206E-2</v>
+        <v>-5.0059059806503381E-2</v>
       </c>
       <c r="J4">
-        <v>0.27164281225738329</v>
+        <v>0.27164281285465708</v>
       </c>
       <c r="K4">
-        <v>0.25218144054202773</v>
+        <v>0.25218144113016083</v>
       </c>
       <c r="L4">
-        <v>-8.2298725560155828E-2</v>
+        <v>-8.2298764589214146E-2</v>
       </c>
       <c r="M4">
-        <v>-0.24633456259909303</v>
+        <v>-0.24633464816111661</v>
       </c>
       <c r="N4">
-        <v>92.143206196455068</v>
+        <v>92.14318897002542</v>
       </c>
       <c r="O4">
-        <v>55.956211366848507</v>
+        <v>55.956211398822617</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1271,46 +1283,46 @@
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>1016.1199727010782</v>
+        <v>1016.1228057023013</v>
       </c>
       <c r="C5">
-        <v>9590237280.4976711</v>
+        <v>9590263817.7452202</v>
       </c>
       <c r="D5">
-        <v>9438095.4396601785</v>
+        <v>9438095.2419592962</v>
       </c>
       <c r="E5">
-        <v>0.4821434765789297</v>
+        <v>0.48214346647941436</v>
       </c>
       <c r="F5">
-        <v>156.67858705635106</v>
+        <v>156.67901464721257</v>
       </c>
       <c r="G5">
-        <v>691.15739482266133</v>
+        <v>691.15933416285611</v>
       </c>
       <c r="H5">
-        <v>1.2101261251179785</v>
+        <v>1.2101247163251214</v>
       </c>
       <c r="I5">
-        <v>-4.3309607927320526E-2</v>
+        <v>-4.3310217984809607E-2</v>
       </c>
       <c r="J5">
-        <v>-0.56713312367111612</v>
+        <v>-0.56713312377867808</v>
       </c>
       <c r="K5">
-        <v>-0.50709822624514778</v>
+        <v>-0.5070982263676278</v>
       </c>
       <c r="L5">
-        <v>8.3028081427743317E-2</v>
+        <v>8.302758032673685E-2</v>
       </c>
       <c r="M5">
-        <v>1.2162327457674529</v>
+        <v>1.2162311488234776</v>
       </c>
       <c r="N5">
-        <v>96.998870088000416</v>
+        <v>96.998860741022995</v>
       </c>
       <c r="O5">
-        <v>44.003088624797613</v>
+        <v>44.003088629273883</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1318,46 +1330,46 @@
         <v>2019</v>
       </c>
       <c r="B6">
-        <v>459.75655468388112</v>
+        <v>459.75812957372676</v>
       </c>
       <c r="C6">
-        <v>10024389666.671915</v>
+        <v>10024423797.591</v>
       </c>
       <c r="D6">
-        <v>21803690.593523942</v>
+        <v>21803690.14221745</v>
       </c>
       <c r="E6">
-        <v>0.97817354745151885</v>
+        <v>0.97817352720466799</v>
       </c>
       <c r="F6">
-        <v>144.66715105835806</v>
+        <v>144.66761280441659</v>
       </c>
       <c r="G6">
-        <v>311.86137653756327</v>
+        <v>311.86247631695335</v>
       </c>
       <c r="H6">
-        <v>-2.6066784032476864E-3</v>
+        <v>-2.606138850008155E-3</v>
       </c>
       <c r="I6">
-        <v>1.3900326498015536E-2</v>
+        <v>1.3900875336022356E-2</v>
       </c>
       <c r="J6">
-        <v>1.6550145808913896E-2</v>
+        <v>1.6550146164924229E-2</v>
       </c>
       <c r="K6">
-        <v>1.0367650232698367E-2</v>
+        <v>1.0367650586543542E-2</v>
       </c>
       <c r="L6">
-        <v>5.753828532776728E-3</v>
+        <v>5.754434254367613E-3</v>
       </c>
       <c r="M6">
-        <v>-1.6745752680884518E-3</v>
+        <v>-1.6740644401017635E-3</v>
       </c>
       <c r="N6">
-        <v>101.39003264980155</v>
+        <v>101.39008753360224</v>
       </c>
       <c r="O6">
-        <v>101.65501458089139</v>
+        <v>101.65501461649242</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1365,40 +1377,40 @@
         <v>2018</v>
       </c>
       <c r="B7">
-        <v>460.95812427122047</v>
+        <v>460.95945391485282</v>
       </c>
       <c r="C7">
-        <v>9886957726.2055798</v>
+        <v>9886986037.2383556</v>
       </c>
       <c r="D7">
-        <v>21448711.29419177</v>
+        <v>21448710.84272122</v>
       </c>
       <c r="E7">
-        <v>0.9681362494397312</v>
+        <v>0.9681362290615837</v>
       </c>
       <c r="F7">
-        <v>143.8395231061688</v>
+        <v>143.83989558213409</v>
       </c>
       <c r="G7">
-        <v>312.38448787509338</v>
+        <v>312.38542965634696</v>
       </c>
       <c r="H7">
-        <v>-3.5645247613669828E-2</v>
+        <v>-3.5645011084420641E-2</v>
       </c>
       <c r="I7">
-        <v>1.566648765768841E-2</v>
+        <v>1.5666737236474937E-2</v>
       </c>
       <c r="J7">
-        <v>5.3208360454890302E-2</v>
+        <v>5.3208360936252141E-2</v>
       </c>
       <c r="K7">
-        <v>4.924647508858393E-2</v>
+        <v>4.9246475568134995E-2</v>
       </c>
       <c r="L7">
-        <v>4.1615133750116939E-6</v>
+        <v>4.0143346826670978E-6</v>
       </c>
       <c r="M7">
-        <v>-3.0183232751069267E-2</v>
+        <v>-3.0182812687121863E-2</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1621,7 +1633,7 @@
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="4" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
202412 December full release"
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BB22FD-F332-496C-B80E-FDCDA4CB0993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A847A67F-A04D-4027-AB32-A1C8D18B20F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>year_data</t>
   </si>
@@ -195,7 +195,10 @@
     <t>HASP</t>
   </si>
   <si>
-    <t>AirNav Ireland</t>
+    <t>Airnav Ireland</t>
+  </si>
+  <si>
+    <t>IAA</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -660,6 +663,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -705,13 +719,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1070,7 +1085,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:O7"/>
+      <selection activeCell="A2" sqref="A2:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,278 +1139,278 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B2">
-        <v>470.26551030000002</v>
+        <v>459.75620180305265</v>
       </c>
       <c r="C2">
-        <v>8923563036</v>
+        <v>9697483659.9791355</v>
       </c>
       <c r="D2">
-        <v>18975584.73</v>
+        <v>21092665.247250497</v>
       </c>
       <c r="E2">
-        <v>0.88557406599999999</v>
+        <v>0.96697865414991746</v>
       </c>
       <c r="F2">
-        <v>133.29054529999999</v>
+        <v>143.54928009986031</v>
       </c>
       <c r="G2">
-        <v>319.75235679999997</v>
+        <v>311.30485855591945</v>
       </c>
       <c r="H2">
-        <v>-0.34658558099999998</v>
+        <v>-7.340211528671825E-2</v>
       </c>
       <c r="I2">
-        <v>3.4281998000000001E-2</v>
+        <v>2.8814621788030959E-2</v>
       </c>
       <c r="J2">
-        <v>0.58288823599999995</v>
+        <v>0.11031401944801345</v>
       </c>
       <c r="K2">
-        <v>0.46956072599999998</v>
+        <v>8.9995961984757455E-2</v>
       </c>
       <c r="L2">
-        <v>-2.3923535999999999E-2</v>
+        <v>2.1593707224610625E-2</v>
       </c>
       <c r="M2">
-        <v>-0.35154045499999997</v>
+        <v>-7.8394847778735288E-2</v>
       </c>
       <c r="N2">
-        <v>96.950101239999995</v>
+        <v>98.083315010808363</v>
       </c>
       <c r="O2">
-        <v>93.290669390000005</v>
+        <v>98.3400140079209</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B3">
-        <v>719.70482509999999</v>
+        <v>496.17661489192318</v>
       </c>
       <c r="C3">
-        <v>8627785321</v>
+        <v>9425880478.9587555</v>
       </c>
       <c r="D3">
-        <v>11987949.810000001</v>
+        <v>18997026.85708373</v>
       </c>
       <c r="E3">
-        <v>0.60261141299999998</v>
+        <v>0.88713966645267239</v>
       </c>
       <c r="F3">
-        <v>136.55748320000001</v>
+        <v>140.51503947674487</v>
       </c>
       <c r="G3">
-        <v>493.09530489999997</v>
+        <v>337.7855015302469</v>
       </c>
       <c r="H3">
-        <v>-0.25295200800000001</v>
+        <v>-0.34632988644957596</v>
       </c>
       <c r="I3">
-        <v>-4.9996459E-2</v>
+        <v>3.4653113848693406E-2</v>
       </c>
       <c r="J3">
-        <v>0.27167672100000001</v>
+        <v>0.58283680468264287</v>
       </c>
       <c r="K3">
-        <v>0.25134547499999998</v>
+        <v>0.46942846814114647</v>
       </c>
       <c r="L3">
-        <v>-8.2098113E-2</v>
+        <v>-2.2738787926019133E-2</v>
       </c>
       <c r="M3">
-        <v>-0.246572025</v>
+        <v>-0.35153837951542866</v>
       </c>
       <c r="N3">
-        <v>93.736622569999994</v>
+        <v>95.336237387785403</v>
       </c>
       <c r="O3">
-        <v>58.936990790000003</v>
+        <v>88.569550852658878</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B4">
-        <v>963.39837990000001</v>
+        <v>759.06272079188182</v>
       </c>
       <c r="C4">
-        <v>9081845434</v>
+        <v>9110184227.7325668</v>
       </c>
       <c r="D4">
-        <v>9426884.6850000005</v>
+        <v>12001885.981475275</v>
       </c>
       <c r="E4">
-        <v>0.48157077700000001</v>
+        <v>0.60373110068768443</v>
       </c>
       <c r="F4">
-        <v>148.77132850000001</v>
+        <v>143.78452530469158</v>
       </c>
       <c r="G4">
-        <v>654.46906869999998</v>
+        <v>520.90284275857732</v>
       </c>
       <c r="H4">
-        <v>1.213430842</v>
+        <v>-0.25298131630137988</v>
       </c>
       <c r="I4">
-        <v>-4.1892621999999997E-2</v>
+        <v>-5.0059059806503381E-2</v>
       </c>
       <c r="J4">
-        <v>-0.56713922999999999</v>
+        <v>0.27164281285465708</v>
       </c>
       <c r="K4">
-        <v>-0.50710518000000004</v>
+        <v>0.25218144113016083</v>
       </c>
       <c r="L4">
-        <v>8.4551656000000003E-2</v>
+        <v>-8.2298764589214146E-2</v>
       </c>
       <c r="M4">
-        <v>1.219649314</v>
+        <v>-0.24633464816111661</v>
       </c>
       <c r="N4">
-        <v>98.669761249999993</v>
+        <v>92.14318897002542</v>
       </c>
       <c r="O4">
-        <v>46.34589106</v>
+        <v>55.956211398822617</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B5">
-        <v>435.25117729999999</v>
+        <v>1016.1228057023013</v>
       </c>
       <c r="C5">
-        <v>9478943216</v>
+        <v>9590263817.7452202</v>
       </c>
       <c r="D5">
-        <v>21778098.969999999</v>
+        <v>9438095.2419592962</v>
       </c>
       <c r="E5">
-        <v>0.977025437</v>
+        <v>0.48214346647941436</v>
       </c>
       <c r="F5">
-        <v>137.1731145</v>
+        <v>156.67901464721257</v>
       </c>
       <c r="G5">
-        <v>294.85246369999999</v>
+        <v>691.15933416285611</v>
       </c>
       <c r="H5">
-        <v>-2.038008E-3</v>
+        <v>1.2101247163251214</v>
       </c>
       <c r="I5">
-        <v>1.4498578999999999E-2</v>
+        <v>-4.3310217984809607E-2</v>
       </c>
       <c r="J5">
-        <v>1.6570358E-2</v>
+        <v>-0.56713312377867808</v>
       </c>
       <c r="K5">
-        <v>1.0387739E-2</v>
+        <v>-0.5070982263676278</v>
       </c>
       <c r="L5">
-        <v>6.3813330000000003E-3</v>
+        <v>8.302758032673685E-2</v>
       </c>
       <c r="M5">
-        <v>-1.1177139999999999E-3</v>
+        <v>1.2162311488234776</v>
       </c>
       <c r="N5">
-        <v>102.9840324</v>
+        <v>96.998860741022995</v>
       </c>
       <c r="O5">
-        <v>107.0688182</v>
+        <v>44.003088629273883</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B6">
-        <v>436.1400342</v>
+        <v>459.75812957372676</v>
       </c>
       <c r="C6">
-        <v>9343476090</v>
+        <v>10024423797.591</v>
       </c>
       <c r="D6">
-        <v>21423110.370000001</v>
+        <v>21803690.14221745</v>
       </c>
       <c r="E6">
-        <v>0.96698069399999997</v>
+        <v>0.97817352720466799</v>
       </c>
       <c r="F6">
-        <v>136.30331770000001</v>
+        <v>144.66761280441659</v>
       </c>
       <c r="G6">
-        <v>295.18239299999999</v>
+        <v>311.86247631695335</v>
       </c>
       <c r="H6">
-        <v>-3.6186771999999999E-2</v>
+        <v>-2.606138850008155E-3</v>
       </c>
       <c r="I6">
-        <v>1.5122490000000001E-2</v>
+        <v>1.3900875336022356E-2</v>
       </c>
       <c r="J6">
-        <v>5.3235690000000002E-2</v>
+        <v>1.6550146164924229E-2</v>
       </c>
       <c r="K6">
-        <v>4.9273702000000003E-2</v>
+        <v>1.0367650586543542E-2</v>
       </c>
       <c r="L6">
-        <v>-1.7275999999999999E-4</v>
+        <v>5.754434254367613E-3</v>
       </c>
       <c r="M6">
-        <v>-3.0874655000000001E-2</v>
+        <v>-1.6740644401017635E-3</v>
       </c>
       <c r="N6">
-        <v>101.512249</v>
+        <v>101.39008753360224</v>
       </c>
       <c r="O6">
-        <v>105.32356900000001</v>
+        <v>101.65501461649242</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B7">
-        <v>452.51509479999999</v>
+        <v>460.95945391485282</v>
       </c>
       <c r="C7">
-        <v>9204284392</v>
+        <v>9886986037.2383556</v>
       </c>
       <c r="D7">
-        <v>20340281.460000001</v>
+        <v>21448710.84272122</v>
       </c>
       <c r="E7">
-        <v>0.92157145699999998</v>
+        <v>0.9681362290615837</v>
       </c>
       <c r="F7">
-        <v>136.32686949999999</v>
+        <v>143.83989558213409</v>
       </c>
       <c r="G7">
-        <v>304.58639269999998</v>
+        <v>312.38542965634696</v>
       </c>
       <c r="H7">
-        <v>-3.5869579999999998E-2</v>
+        <v>-3.5645011084420641E-2</v>
       </c>
       <c r="I7">
-        <v>8.9638819999999994E-3</v>
+        <v>1.5666737236474937E-2</v>
       </c>
       <c r="J7">
-        <v>4.6501449E-2</v>
+        <v>5.3208360936252141E-2</v>
       </c>
       <c r="K7">
-        <v>4.3322938999999998E-2</v>
+        <v>4.9246475568134995E-2</v>
       </c>
       <c r="L7">
-        <v>1.2469209E-2</v>
+        <v>4.0143346826670978E-6</v>
       </c>
       <c r="M7">
-        <v>-3.8898467999999999E-2</v>
+        <v>-3.0182812687121863E-2</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1411,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,191 +1444,196 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated ACE landing page
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A847A67F-A04D-4027-AB32-A1C8D18B20F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCAF000-B8EB-41EE-B7B0-D7783079BDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -1084,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:O7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,46 +1142,46 @@
         <v>2023</v>
       </c>
       <c r="B2">
-        <v>459.75620180305265</v>
+        <v>459.51125496142458</v>
       </c>
       <c r="C2">
-        <v>9697483659.9791355</v>
+        <v>9696014411.1017056</v>
       </c>
       <c r="D2">
-        <v>21092665.247250497</v>
+        <v>21100711.476404805</v>
       </c>
       <c r="E2">
-        <v>0.96697865414991746</v>
+        <v>0.93449148017114469</v>
       </c>
       <c r="F2">
-        <v>143.54928009986031</v>
+        <v>141.76294716186041</v>
       </c>
       <c r="G2">
-        <v>311.30485855591945</v>
+        <v>307.81062400875106</v>
       </c>
       <c r="H2">
-        <v>-7.340211528671825E-2</v>
+        <v>-7.3924857539470756E-2</v>
       </c>
       <c r="I2">
-        <v>2.8814621788030959E-2</v>
+        <v>2.8658747874637847E-2</v>
       </c>
       <c r="J2">
-        <v>0.11031401944801345</v>
+        <v>0.11077244244084761</v>
       </c>
       <c r="K2">
-        <v>8.9995961984757455E-2</v>
+        <v>8.8513109734926765E-2</v>
       </c>
       <c r="L2">
-        <v>2.1593707224610625E-2</v>
+        <v>2.0863303800442878E-2</v>
       </c>
       <c r="M2">
-        <v>-7.8394847778735288E-2</v>
+        <v>-7.9620411780101707E-2</v>
       </c>
       <c r="N2">
-        <v>98.083315010808363</v>
+        <v>98.068454578398587</v>
       </c>
       <c r="O2">
-        <v>98.3400140079209</v>
+        <v>98.380793802270077</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1189,46 +1189,46 @@
         <v>2022</v>
       </c>
       <c r="B3">
-        <v>496.17661489192318</v>
+        <v>496.1921920725884</v>
       </c>
       <c r="C3">
         <v>9425880478.9587555</v>
       </c>
       <c r="D3">
-        <v>18997026.85708373</v>
+        <v>18996430.475028183</v>
       </c>
       <c r="E3">
-        <v>0.88713966645267239</v>
+        <v>0.85850273351205741</v>
       </c>
       <c r="F3">
-        <v>140.51503947674487</v>
+        <v>138.86574885600163</v>
       </c>
       <c r="G3">
-        <v>337.7855015302469</v>
+        <v>334.43877716159056</v>
       </c>
       <c r="H3">
-        <v>-0.34632988644957596</v>
+        <v>-0.34633047653699467</v>
       </c>
       <c r="I3">
         <v>3.4653113848693406E-2</v>
       </c>
       <c r="J3">
-        <v>0.58283680468264287</v>
+        <v>0.58283823355771003</v>
       </c>
       <c r="K3">
-        <v>0.46942846814114647</v>
+        <v>0.42204113678545663</v>
       </c>
       <c r="L3">
-        <v>-2.2738787926019133E-2</v>
+        <v>-3.4209359027104091E-2</v>
       </c>
       <c r="M3">
-        <v>-0.35153837951542866</v>
+        <v>-0.35798396816584188</v>
       </c>
       <c r="N3">
-        <v>95.336237387785403</v>
+        <v>95.336237387785417</v>
       </c>
       <c r="O3">
-        <v>88.569550852658878</v>
+        <v>88.569710629555161</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1236,46 +1236,46 @@
         <v>2021</v>
       </c>
       <c r="B4">
-        <v>759.06272079188182</v>
+        <v>759.08723638187269</v>
       </c>
       <c r="C4">
-        <v>9110184227.7325668</v>
+        <v>9110184227.7325687</v>
       </c>
       <c r="D4">
-        <v>12001885.981475275</v>
+        <v>12001498.366848476</v>
       </c>
       <c r="E4">
-        <v>0.60373110068768443</v>
+        <v>0.6037116025016791</v>
       </c>
       <c r="F4">
-        <v>143.78452530469158</v>
+        <v>143.78452530469156</v>
       </c>
       <c r="G4">
-        <v>520.90284275857732</v>
+        <v>520.91966645465459</v>
       </c>
       <c r="H4">
-        <v>-0.25298131630137988</v>
+        <v>-0.25298186968904457</v>
       </c>
       <c r="I4">
-        <v>-5.0059059806503381E-2</v>
+        <v>-5.0059059806503159E-2</v>
       </c>
       <c r="J4">
-        <v>0.27164281285465708</v>
+        <v>0.27164375488192261</v>
       </c>
       <c r="K4">
-        <v>0.25218144113016083</v>
+        <v>0.25218236874053002</v>
       </c>
       <c r="L4">
-        <v>-8.2298764589214146E-2</v>
+        <v>-8.2298764589214035E-2</v>
       </c>
       <c r="M4">
-        <v>-0.24633464816111661</v>
+        <v>-0.24633520647259943</v>
       </c>
       <c r="N4">
-        <v>92.14318897002542</v>
+        <v>92.143188970025463</v>
       </c>
       <c r="O4">
-        <v>55.956211398822617</v>
+        <v>55.956261828777663</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1283,46 +1283,46 @@
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>1016.1228057023013</v>
+        <v>1016.1563763732124</v>
       </c>
       <c r="C5">
         <v>9590263817.7452202</v>
       </c>
       <c r="D5">
-        <v>9438095.2419592962</v>
+        <v>9437783.4364175871</v>
       </c>
       <c r="E5">
-        <v>0.48214346647941436</v>
+        <v>0.48212753794713165</v>
       </c>
       <c r="F5">
-        <v>156.67901464721257</v>
+        <v>156.67901464721251</v>
       </c>
       <c r="G5">
-        <v>691.15933416285611</v>
+        <v>691.18216868878562</v>
       </c>
       <c r="H5">
-        <v>1.2101247163251214</v>
+        <v>1.2101255825117465</v>
       </c>
       <c r="I5">
-        <v>-4.3310217984809607E-2</v>
+        <v>-4.3310217984809829E-2</v>
       </c>
       <c r="J5">
-        <v>-0.56713312377867808</v>
+        <v>-0.5671332934267298</v>
       </c>
       <c r="K5">
-        <v>-0.5070982263676278</v>
+        <v>-0.50709841954439916</v>
       </c>
       <c r="L5">
         <v>8.302758032673685E-2</v>
       </c>
       <c r="M5">
-        <v>1.2162311488234776</v>
+        <v>1.2162320174033208</v>
       </c>
       <c r="N5">
-        <v>96.998860741022995</v>
+        <v>96.998860741023009</v>
       </c>
       <c r="O5">
-        <v>44.003088629273883</v>
+        <v>44.003095689306029</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1330,46 +1330,46 @@
         <v>2019</v>
       </c>
       <c r="B6">
-        <v>459.75812957372676</v>
+        <v>459.77313887221686</v>
       </c>
       <c r="C6">
-        <v>10024423797.591</v>
+        <v>10024423797.591002</v>
       </c>
       <c r="D6">
-        <v>21803690.14221745</v>
+        <v>21802978.360545449</v>
       </c>
       <c r="E6">
-        <v>0.97817352720466799</v>
+        <v>0.97814159472057183</v>
       </c>
       <c r="F6">
-        <v>144.66761280441659</v>
+        <v>144.66761280441656</v>
       </c>
       <c r="G6">
-        <v>311.86247631695335</v>
+        <v>311.87265740281964</v>
       </c>
       <c r="H6">
-        <v>-2.606138850008155E-3</v>
+        <v>-2.6066897717813564E-3</v>
       </c>
       <c r="I6">
-        <v>1.3900875336022356E-2</v>
+        <v>1.39008753360228E-2</v>
       </c>
       <c r="J6">
-        <v>1.6550146164924229E-2</v>
+        <v>1.655070766819855E-2</v>
       </c>
       <c r="K6">
-        <v>1.0367650586543542E-2</v>
+        <v>1.0368208674844448E-2</v>
       </c>
       <c r="L6">
         <v>5.754434254367613E-3</v>
       </c>
       <c r="M6">
-        <v>-1.6740644401017635E-3</v>
+        <v>-1.6746158767168007E-3</v>
       </c>
       <c r="N6">
-        <v>101.39008753360224</v>
+        <v>101.39008753360228</v>
       </c>
       <c r="O6">
-        <v>101.65501461649242</v>
+        <v>101.65507076681986</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1377,40 +1377,40 @@
         <v>2018</v>
       </c>
       <c r="B7">
-        <v>460.95945391485282</v>
+        <v>460.97475705648537</v>
       </c>
       <c r="C7">
-        <v>9886986037.2383556</v>
+        <v>9886986037.2383537</v>
       </c>
       <c r="D7">
-        <v>21448710.84272122</v>
+        <v>21447998.802300699</v>
       </c>
       <c r="E7">
-        <v>0.9681362290615837</v>
+        <v>0.9681040895016485</v>
       </c>
       <c r="F7">
-        <v>143.83989558213409</v>
+        <v>143.83989558213406</v>
       </c>
       <c r="G7">
-        <v>312.38542965634696</v>
+        <v>312.3958003699388</v>
       </c>
       <c r="H7">
-        <v>-3.5645011084420641E-2</v>
+        <v>-3.564570624302521E-2</v>
       </c>
       <c r="I7">
-        <v>1.5666737236474937E-2</v>
+        <v>1.5666737236474715E-2</v>
       </c>
       <c r="J7">
-        <v>5.3208360936252141E-2</v>
+        <v>5.3209120145662148E-2</v>
       </c>
       <c r="K7">
-        <v>4.9246475568134995E-2</v>
+        <v>4.9247231921604406E-2</v>
       </c>
       <c r="L7">
         <v>4.0143346826670978E-6</v>
       </c>
       <c r="M7">
-        <v>-3.0182812687121863E-2</v>
+        <v>-3.0183511783170802E-2</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1428,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,4 +1640,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{fd60f3b8-f236-4830-aecc-da0a7fc54679}" enabled="1" method="Standard" siteId="{76f33c20-5979-4408-adf7-8b3c4be95e52}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
reordered ace ansp list and added uskatse
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCAF000-B8EB-41EE-B7B0-D7783079BDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CB8E00-2301-4597-AE4B-B269D413B715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -198,14 +198,14 @@
     <t>Airnav Ireland</t>
   </si>
   <si>
-    <t>IAA</t>
+    <t>UkSATSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +344,12 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -719,7 +725,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -727,6 +733,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1084,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:O7"/>
     </sheetView>
   </sheetViews>
@@ -1428,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,102 +1546,102 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>49</v>
+      <c r="A39" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>50</v>
+      <c r="A40" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected typo AirNav Ireland
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CB8E00-2301-4597-AE4B-B269D413B715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BD4D9F-01E3-4EF8-99DC-13F08F4A9F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,10 +195,10 @@
     <t>HASP</t>
   </si>
   <si>
-    <t>Airnav Ireland</t>
-  </si>
-  <si>
     <t>UkSATSE</t>
+  </si>
+  <si>
+    <t>AirNav Ireland</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1436,7 @@
   <dimension ref="A1:A40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1641,7 +1641,7 @@
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
202506 June full release
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A847A67F-A04D-4027-AB32-A1C8D18B20F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BD4D9F-01E3-4EF8-99DC-13F08F4A9F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -195,17 +195,17 @@
     <t>HASP</t>
   </si>
   <si>
-    <t>Airnav Ireland</t>
-  </si>
-  <si>
-    <t>IAA</t>
+    <t>UkSATSE</t>
+  </si>
+  <si>
+    <t>AirNav Ireland</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +344,12 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -719,7 +725,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -727,6 +733,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1085,7 +1092,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:O7"/>
+      <selection activeCell="B2" sqref="B2:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,46 +1149,46 @@
         <v>2023</v>
       </c>
       <c r="B2">
-        <v>459.75620180305265</v>
+        <v>459.51125496142458</v>
       </c>
       <c r="C2">
-        <v>9697483659.9791355</v>
+        <v>9696014411.1017056</v>
       </c>
       <c r="D2">
-        <v>21092665.247250497</v>
+        <v>21100711.476404805</v>
       </c>
       <c r="E2">
-        <v>0.96697865414991746</v>
+        <v>0.93449148017114469</v>
       </c>
       <c r="F2">
-        <v>143.54928009986031</v>
+        <v>141.76294716186041</v>
       </c>
       <c r="G2">
-        <v>311.30485855591945</v>
+        <v>307.81062400875106</v>
       </c>
       <c r="H2">
-        <v>-7.340211528671825E-2</v>
+        <v>-7.3924857539470756E-2</v>
       </c>
       <c r="I2">
-        <v>2.8814621788030959E-2</v>
+        <v>2.8658747874637847E-2</v>
       </c>
       <c r="J2">
-        <v>0.11031401944801345</v>
+        <v>0.11077244244084761</v>
       </c>
       <c r="K2">
-        <v>8.9995961984757455E-2</v>
+        <v>8.8513109734926765E-2</v>
       </c>
       <c r="L2">
-        <v>2.1593707224610625E-2</v>
+        <v>2.0863303800442878E-2</v>
       </c>
       <c r="M2">
-        <v>-7.8394847778735288E-2</v>
+        <v>-7.9620411780101707E-2</v>
       </c>
       <c r="N2">
-        <v>98.083315010808363</v>
+        <v>98.068454578398587</v>
       </c>
       <c r="O2">
-        <v>98.3400140079209</v>
+        <v>98.380793802270077</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1189,46 +1196,46 @@
         <v>2022</v>
       </c>
       <c r="B3">
-        <v>496.17661489192318</v>
+        <v>496.1921920725884</v>
       </c>
       <c r="C3">
         <v>9425880478.9587555</v>
       </c>
       <c r="D3">
-        <v>18997026.85708373</v>
+        <v>18996430.475028183</v>
       </c>
       <c r="E3">
-        <v>0.88713966645267239</v>
+        <v>0.85850273351205741</v>
       </c>
       <c r="F3">
-        <v>140.51503947674487</v>
+        <v>138.86574885600163</v>
       </c>
       <c r="G3">
-        <v>337.7855015302469</v>
+        <v>334.43877716159056</v>
       </c>
       <c r="H3">
-        <v>-0.34632988644957596</v>
+        <v>-0.34633047653699467</v>
       </c>
       <c r="I3">
         <v>3.4653113848693406E-2</v>
       </c>
       <c r="J3">
-        <v>0.58283680468264287</v>
+        <v>0.58283823355771003</v>
       </c>
       <c r="K3">
-        <v>0.46942846814114647</v>
+        <v>0.42204113678545663</v>
       </c>
       <c r="L3">
-        <v>-2.2738787926019133E-2</v>
+        <v>-3.4209359027104091E-2</v>
       </c>
       <c r="M3">
-        <v>-0.35153837951542866</v>
+        <v>-0.35798396816584188</v>
       </c>
       <c r="N3">
-        <v>95.336237387785403</v>
+        <v>95.336237387785417</v>
       </c>
       <c r="O3">
-        <v>88.569550852658878</v>
+        <v>88.569710629555161</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1236,46 +1243,46 @@
         <v>2021</v>
       </c>
       <c r="B4">
-        <v>759.06272079188182</v>
+        <v>759.08723638187269</v>
       </c>
       <c r="C4">
-        <v>9110184227.7325668</v>
+        <v>9110184227.7325687</v>
       </c>
       <c r="D4">
-        <v>12001885.981475275</v>
+        <v>12001498.366848476</v>
       </c>
       <c r="E4">
-        <v>0.60373110068768443</v>
+        <v>0.6037116025016791</v>
       </c>
       <c r="F4">
-        <v>143.78452530469158</v>
+        <v>143.78452530469156</v>
       </c>
       <c r="G4">
-        <v>520.90284275857732</v>
+        <v>520.91966645465459</v>
       </c>
       <c r="H4">
-        <v>-0.25298131630137988</v>
+        <v>-0.25298186968904457</v>
       </c>
       <c r="I4">
-        <v>-5.0059059806503381E-2</v>
+        <v>-5.0059059806503159E-2</v>
       </c>
       <c r="J4">
-        <v>0.27164281285465708</v>
+        <v>0.27164375488192261</v>
       </c>
       <c r="K4">
-        <v>0.25218144113016083</v>
+        <v>0.25218236874053002</v>
       </c>
       <c r="L4">
-        <v>-8.2298764589214146E-2</v>
+        <v>-8.2298764589214035E-2</v>
       </c>
       <c r="M4">
-        <v>-0.24633464816111661</v>
+        <v>-0.24633520647259943</v>
       </c>
       <c r="N4">
-        <v>92.14318897002542</v>
+        <v>92.143188970025463</v>
       </c>
       <c r="O4">
-        <v>55.956211398822617</v>
+        <v>55.956261828777663</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1283,46 +1290,46 @@
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>1016.1228057023013</v>
+        <v>1016.1563763732124</v>
       </c>
       <c r="C5">
         <v>9590263817.7452202</v>
       </c>
       <c r="D5">
-        <v>9438095.2419592962</v>
+        <v>9437783.4364175871</v>
       </c>
       <c r="E5">
-        <v>0.48214346647941436</v>
+        <v>0.48212753794713165</v>
       </c>
       <c r="F5">
-        <v>156.67901464721257</v>
+        <v>156.67901464721251</v>
       </c>
       <c r="G5">
-        <v>691.15933416285611</v>
+        <v>691.18216868878562</v>
       </c>
       <c r="H5">
-        <v>1.2101247163251214</v>
+        <v>1.2101255825117465</v>
       </c>
       <c r="I5">
-        <v>-4.3310217984809607E-2</v>
+        <v>-4.3310217984809829E-2</v>
       </c>
       <c r="J5">
-        <v>-0.56713312377867808</v>
+        <v>-0.5671332934267298</v>
       </c>
       <c r="K5">
-        <v>-0.5070982263676278</v>
+        <v>-0.50709841954439916</v>
       </c>
       <c r="L5">
         <v>8.302758032673685E-2</v>
       </c>
       <c r="M5">
-        <v>1.2162311488234776</v>
+        <v>1.2162320174033208</v>
       </c>
       <c r="N5">
-        <v>96.998860741022995</v>
+        <v>96.998860741023009</v>
       </c>
       <c r="O5">
-        <v>44.003088629273883</v>
+        <v>44.003095689306029</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1330,46 +1337,46 @@
         <v>2019</v>
       </c>
       <c r="B6">
-        <v>459.75812957372676</v>
+        <v>459.77313887221686</v>
       </c>
       <c r="C6">
-        <v>10024423797.591</v>
+        <v>10024423797.591002</v>
       </c>
       <c r="D6">
-        <v>21803690.14221745</v>
+        <v>21802978.360545449</v>
       </c>
       <c r="E6">
-        <v>0.97817352720466799</v>
+        <v>0.97814159472057183</v>
       </c>
       <c r="F6">
-        <v>144.66761280441659</v>
+        <v>144.66761280441656</v>
       </c>
       <c r="G6">
-        <v>311.86247631695335</v>
+        <v>311.87265740281964</v>
       </c>
       <c r="H6">
-        <v>-2.606138850008155E-3</v>
+        <v>-2.6066897717813564E-3</v>
       </c>
       <c r="I6">
-        <v>1.3900875336022356E-2</v>
+        <v>1.39008753360228E-2</v>
       </c>
       <c r="J6">
-        <v>1.6550146164924229E-2</v>
+        <v>1.655070766819855E-2</v>
       </c>
       <c r="K6">
-        <v>1.0367650586543542E-2</v>
+        <v>1.0368208674844448E-2</v>
       </c>
       <c r="L6">
         <v>5.754434254367613E-3</v>
       </c>
       <c r="M6">
-        <v>-1.6740644401017635E-3</v>
+        <v>-1.6746158767168007E-3</v>
       </c>
       <c r="N6">
-        <v>101.39008753360224</v>
+        <v>101.39008753360228</v>
       </c>
       <c r="O6">
-        <v>101.65501461649242</v>
+        <v>101.65507076681986</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1377,40 +1384,40 @@
         <v>2018</v>
       </c>
       <c r="B7">
-        <v>460.95945391485282</v>
+        <v>460.97475705648537</v>
       </c>
       <c r="C7">
-        <v>9886986037.2383556</v>
+        <v>9886986037.2383537</v>
       </c>
       <c r="D7">
-        <v>21448710.84272122</v>
+        <v>21447998.802300699</v>
       </c>
       <c r="E7">
-        <v>0.9681362290615837</v>
+        <v>0.9681040895016485</v>
       </c>
       <c r="F7">
-        <v>143.83989558213409</v>
+        <v>143.83989558213406</v>
       </c>
       <c r="G7">
-        <v>312.38542965634696</v>
+        <v>312.3958003699388</v>
       </c>
       <c r="H7">
-        <v>-3.5645011084420641E-2</v>
+        <v>-3.564570624302521E-2</v>
       </c>
       <c r="I7">
-        <v>1.5666737236474937E-2</v>
+        <v>1.5666737236474715E-2</v>
       </c>
       <c r="J7">
-        <v>5.3208360936252141E-2</v>
+        <v>5.3209120145662148E-2</v>
       </c>
       <c r="K7">
-        <v>4.9246475568134995E-2</v>
+        <v>4.9247231921604406E-2</v>
       </c>
       <c r="L7">
         <v>4.0143346826670978E-6</v>
       </c>
       <c r="M7">
-        <v>-3.0182812687121863E-2</v>
+        <v>-3.0183511783170802E-2</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1428,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1451,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1539,105 +1546,111 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>49</v>
+      <c r="A39" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>50</v>
+      <c r="A40" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{fd60f3b8-f236-4830-aecc-da0a7fc54679}" enabled="1" method="Standard" siteId="{76f33c20-5979-4408-adf7-8b3c4be95e52}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
added ACE hlsr to home and eco landing pages
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BD4D9F-01E3-4EF8-99DC-13F08F4A9F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9174317F-79C5-4BB9-9CD8-36421E4B7C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,278 +1146,278 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B2">
-        <v>459.51125496142458</v>
+        <v>469.4605934329557</v>
       </c>
       <c r="C2">
-        <v>9696014411.1017056</v>
+        <v>10467653125.780624</v>
       </c>
       <c r="D2">
-        <v>21100711.476404805</v>
+        <v>22297192.293042853</v>
       </c>
       <c r="E2">
-        <v>0.93449148017114469</v>
+        <v>0.98081881913019253</v>
       </c>
       <c r="F2">
-        <v>141.76294716186041</v>
+        <v>152.18400188546104</v>
       </c>
       <c r="G2">
-        <v>307.81062400875106</v>
+        <v>314.30043651384142</v>
       </c>
       <c r="H2">
-        <v>-7.3924857539470756E-2</v>
+        <v>-1.3990770346900772E-2</v>
       </c>
       <c r="I2">
-        <v>2.8658747874637847E-2</v>
+        <v>4.0218364367912596E-2</v>
       </c>
       <c r="J2">
-        <v>0.11077244244084761</v>
+        <v>5.4978323817399977E-2</v>
       </c>
       <c r="K2">
-        <v>8.8513109734926765E-2</v>
+        <v>4.7861539125722885E-2</v>
       </c>
       <c r="L2">
-        <v>2.0863303800442878E-2</v>
+        <v>3.8514105249225938E-2</v>
       </c>
       <c r="M2">
-        <v>-7.9620411780101707E-2</v>
+        <v>-1.6474730305083396E-2</v>
       </c>
       <c r="N2">
-        <v>98.068454578398587</v>
+        <v>100.98603190277626</v>
       </c>
       <c r="O2">
-        <v>98.380793802270077</v>
+        <v>102.09317864913423</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B3">
-        <v>496.1921920725884</v>
+        <v>476.12190567234626</v>
       </c>
       <c r="C3">
-        <v>9425880478.9587555</v>
+        <v>10062938210.229813</v>
       </c>
       <c r="D3">
-        <v>18996430.475028183</v>
+        <v>21135213.671842363</v>
       </c>
       <c r="E3">
-        <v>0.85850273351205741</v>
+        <v>0.93601948588411121</v>
       </c>
       <c r="F3">
-        <v>138.86574885600163</v>
+        <v>146.54013952842695</v>
       </c>
       <c r="G3">
-        <v>334.43877716159056</v>
+        <v>319.56518678095119</v>
       </c>
       <c r="H3">
-        <v>-0.34633047653699467</v>
+        <v>-7.2964061904103206E-2</v>
       </c>
       <c r="I3">
-        <v>3.4653113848693406E-2</v>
+        <v>2.9726379638513656E-2</v>
       </c>
       <c r="J3">
-        <v>0.58283823355771003</v>
+        <v>0.11077288088047554</v>
       </c>
       <c r="K3">
-        <v>0.42204113678545663</v>
+        <v>8.8513539388441087E-2</v>
       </c>
       <c r="L3">
-        <v>-3.4209359027104091E-2</v>
+        <v>2.1614143908957439E-2</v>
       </c>
       <c r="M3">
-        <v>-0.35798396816584188</v>
+        <v>-7.8497934256253843E-2</v>
       </c>
       <c r="N3">
-        <v>95.336237387785417</v>
+        <v>97.081569949152268</v>
       </c>
       <c r="O3">
-        <v>88.569710629555161</v>
+        <v>96.772773756823597</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B4">
-        <v>759.08723638187269</v>
+        <v>513.59595254773615</v>
       </c>
       <c r="C4">
-        <v>9110184227.7325687</v>
+        <v>9772438979.1416397</v>
       </c>
       <c r="D4">
-        <v>12001498.366848476</v>
+        <v>19027484.408053901</v>
       </c>
       <c r="E4">
-        <v>0.6037116025016791</v>
+        <v>0.85990614908657403</v>
       </c>
       <c r="F4">
-        <v>143.78452530469156</v>
+        <v>143.43981081519371</v>
       </c>
       <c r="G4">
-        <v>520.91966645465459</v>
+        <v>346.78727119621755</v>
       </c>
       <c r="H4">
-        <v>-0.25298186968904457</v>
+        <v>-0.34491825017192079</v>
       </c>
       <c r="I4">
-        <v>-5.0059059806503159E-2</v>
+        <v>3.6839780409229528E-2</v>
       </c>
       <c r="J4">
-        <v>0.27164375488192261</v>
+        <v>0.58276395378338597</v>
       </c>
       <c r="K4">
-        <v>0.25218236874053002</v>
+        <v>0.42197440293200161</v>
       </c>
       <c r="L4">
-        <v>-8.2298764589214035E-2</v>
+        <v>-3.3503681179227307E-2</v>
       </c>
       <c r="M4">
-        <v>-0.24633520647259943</v>
+        <v>-0.35612961410659494</v>
       </c>
       <c r="N4">
-        <v>92.143188970025463</v>
+        <v>94.278996701272078</v>
       </c>
       <c r="O4">
-        <v>55.956261828777663</v>
+        <v>87.122016951039342</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B5">
-        <v>1016.1563763732124</v>
+        <v>784.01810565250082</v>
       </c>
       <c r="C5">
-        <v>9590263817.7452202</v>
+        <v>9425216088.144846</v>
       </c>
       <c r="D5">
-        <v>9437783.4364175871</v>
+        <v>12021681.668053685</v>
       </c>
       <c r="E5">
-        <v>0.48212753794713165</v>
+        <v>0.6047268834892624</v>
       </c>
       <c r="F5">
-        <v>156.67901464721251</v>
+        <v>148.41216466318815</v>
       </c>
       <c r="G5">
-        <v>691.18216868878562</v>
+        <v>538.59795200090059</v>
       </c>
       <c r="H5">
-        <v>1.2101255825117465</v>
+        <v>-0.25272924176920852</v>
       </c>
       <c r="I5">
-        <v>-4.3310217984809829E-2</v>
+        <v>-4.9774400373029382E-2</v>
       </c>
       <c r="J5">
-        <v>-0.5671332934267298</v>
+        <v>0.27159478563925998</v>
       </c>
       <c r="K5">
-        <v>-0.50709841954439916</v>
+        <v>0.25213414892893815</v>
       </c>
       <c r="L5">
-        <v>8.302758032673685E-2</v>
+        <v>-8.2604403998122189E-2</v>
       </c>
       <c r="M5">
-        <v>1.2162320174033208</v>
+        <v>-0.24587929212811932</v>
       </c>
       <c r="N5">
-        <v>96.998860741023009</v>
+        <v>90.929185475562264</v>
       </c>
       <c r="O5">
-        <v>44.003095689306029</v>
+        <v>55.044226110144713</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B6">
-        <v>459.77313887221686</v>
+        <v>1049.1754120135931</v>
       </c>
       <c r="C6">
-        <v>10024423797.591002</v>
+        <v>9918924613.1075573</v>
       </c>
       <c r="D6">
-        <v>21802978.360545449</v>
+        <v>9454019.3179622926</v>
       </c>
       <c r="E6">
-        <v>0.97814159472057183</v>
+        <v>0.48295694515363163</v>
       </c>
       <c r="F6">
-        <v>144.66761280441656</v>
+        <v>161.77553643159669</v>
       </c>
       <c r="G6">
-        <v>311.87265740281964</v>
+        <v>714.20655390940976</v>
       </c>
       <c r="H6">
-        <v>-2.6066897717813564E-3</v>
+        <v>1.210617188802134</v>
       </c>
       <c r="I6">
-        <v>1.39008753360228E-2</v>
+        <v>-4.3077922640073374E-2</v>
       </c>
       <c r="J6">
-        <v>1.655070766819855E-2</v>
+        <v>-0.56712447446477454</v>
       </c>
       <c r="K6">
-        <v>1.0368208674844448E-2</v>
+        <v>-0.50708837746858282</v>
       </c>
       <c r="L6">
-        <v>5.754434254367613E-3</v>
+        <v>8.3696161698424421E-2</v>
       </c>
       <c r="M6">
-        <v>-1.6746158767168007E-3</v>
+        <v>1.2163174140894872</v>
       </c>
       <c r="N6">
-        <v>101.39008753360228</v>
+        <v>95.692207735992667</v>
       </c>
       <c r="O6">
-        <v>101.65507076681986</v>
+        <v>43.287552553522552</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B7">
-        <v>460.97475705648537</v>
+        <v>474.60746135883858</v>
       </c>
       <c r="C7">
-        <v>9886986037.2383537</v>
+        <v>10365446516.265041</v>
       </c>
       <c r="D7">
-        <v>21447998.802300699</v>
+        <v>21840041.213401809</v>
       </c>
       <c r="E7">
-        <v>0.9681040895016485</v>
+        <v>0.97980433626891994</v>
       </c>
       <c r="F7">
-        <v>143.83989558213406</v>
+        <v>149.2812673416262</v>
       </c>
       <c r="G7">
-        <v>312.3958003699388</v>
+        <v>322.2492181711354</v>
       </c>
       <c r="H7">
-        <v>-3.564570624302521E-2</v>
+        <v>-2.3237134232800827E-3</v>
       </c>
       <c r="I7">
-        <v>1.5666737236474715E-2</v>
+        <v>1.4159414678369009E-2</v>
       </c>
       <c r="J7">
-        <v>5.3209120145662148E-2</v>
+        <v>1.6521519378000837E-2</v>
       </c>
       <c r="K7">
-        <v>4.9247231921604406E-2</v>
+        <v>1.0339197903164399E-2</v>
       </c>
       <c r="L7">
-        <v>4.0143346826670978E-6</v>
+        <v>5.633255473421972E-3</v>
       </c>
       <c r="M7">
-        <v>-3.0183511783170802E-2</v>
+        <v>-1.2163576101731355E-3</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1435,9 +1435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Updates to ACE landing page
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9174317F-79C5-4BB9-9CD8-36421E4B7C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8254106-DBCF-432D-BC27-E34568B91154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="A2" sqref="A2:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
202512 December full release
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\aiu-portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BD4D9F-01E3-4EF8-99DC-13F08F4A9F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8254106-DBCF-432D-BC27-E34568B91154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,278 +1146,278 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B2">
-        <v>459.51125496142458</v>
+        <v>469.4605934329557</v>
       </c>
       <c r="C2">
-        <v>9696014411.1017056</v>
+        <v>10467653125.780624</v>
       </c>
       <c r="D2">
-        <v>21100711.476404805</v>
+        <v>22297192.293042853</v>
       </c>
       <c r="E2">
-        <v>0.93449148017114469</v>
+        <v>0.98081881913019253</v>
       </c>
       <c r="F2">
-        <v>141.76294716186041</v>
+        <v>152.18400188546104</v>
       </c>
       <c r="G2">
-        <v>307.81062400875106</v>
+        <v>314.30043651384142</v>
       </c>
       <c r="H2">
-        <v>-7.3924857539470756E-2</v>
+        <v>-1.3990770346900772E-2</v>
       </c>
       <c r="I2">
-        <v>2.8658747874637847E-2</v>
+        <v>4.0218364367912596E-2</v>
       </c>
       <c r="J2">
-        <v>0.11077244244084761</v>
+        <v>5.4978323817399977E-2</v>
       </c>
       <c r="K2">
-        <v>8.8513109734926765E-2</v>
+        <v>4.7861539125722885E-2</v>
       </c>
       <c r="L2">
-        <v>2.0863303800442878E-2</v>
+        <v>3.8514105249225938E-2</v>
       </c>
       <c r="M2">
-        <v>-7.9620411780101707E-2</v>
+        <v>-1.6474730305083396E-2</v>
       </c>
       <c r="N2">
-        <v>98.068454578398587</v>
+        <v>100.98603190277626</v>
       </c>
       <c r="O2">
-        <v>98.380793802270077</v>
+        <v>102.09317864913423</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B3">
-        <v>496.1921920725884</v>
+        <v>476.12190567234626</v>
       </c>
       <c r="C3">
-        <v>9425880478.9587555</v>
+        <v>10062938210.229813</v>
       </c>
       <c r="D3">
-        <v>18996430.475028183</v>
+        <v>21135213.671842363</v>
       </c>
       <c r="E3">
-        <v>0.85850273351205741</v>
+        <v>0.93601948588411121</v>
       </c>
       <c r="F3">
-        <v>138.86574885600163</v>
+        <v>146.54013952842695</v>
       </c>
       <c r="G3">
-        <v>334.43877716159056</v>
+        <v>319.56518678095119</v>
       </c>
       <c r="H3">
-        <v>-0.34633047653699467</v>
+        <v>-7.2964061904103206E-2</v>
       </c>
       <c r="I3">
-        <v>3.4653113848693406E-2</v>
+        <v>2.9726379638513656E-2</v>
       </c>
       <c r="J3">
-        <v>0.58283823355771003</v>
+        <v>0.11077288088047554</v>
       </c>
       <c r="K3">
-        <v>0.42204113678545663</v>
+        <v>8.8513539388441087E-2</v>
       </c>
       <c r="L3">
-        <v>-3.4209359027104091E-2</v>
+        <v>2.1614143908957439E-2</v>
       </c>
       <c r="M3">
-        <v>-0.35798396816584188</v>
+        <v>-7.8497934256253843E-2</v>
       </c>
       <c r="N3">
-        <v>95.336237387785417</v>
+        <v>97.081569949152268</v>
       </c>
       <c r="O3">
-        <v>88.569710629555161</v>
+        <v>96.772773756823597</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B4">
-        <v>759.08723638187269</v>
+        <v>513.59595254773615</v>
       </c>
       <c r="C4">
-        <v>9110184227.7325687</v>
+        <v>9772438979.1416397</v>
       </c>
       <c r="D4">
-        <v>12001498.366848476</v>
+        <v>19027484.408053901</v>
       </c>
       <c r="E4">
-        <v>0.6037116025016791</v>
+        <v>0.85990614908657403</v>
       </c>
       <c r="F4">
-        <v>143.78452530469156</v>
+        <v>143.43981081519371</v>
       </c>
       <c r="G4">
-        <v>520.91966645465459</v>
+        <v>346.78727119621755</v>
       </c>
       <c r="H4">
-        <v>-0.25298186968904457</v>
+        <v>-0.34491825017192079</v>
       </c>
       <c r="I4">
-        <v>-5.0059059806503159E-2</v>
+        <v>3.6839780409229528E-2</v>
       </c>
       <c r="J4">
-        <v>0.27164375488192261</v>
+        <v>0.58276395378338597</v>
       </c>
       <c r="K4">
-        <v>0.25218236874053002</v>
+        <v>0.42197440293200161</v>
       </c>
       <c r="L4">
-        <v>-8.2298764589214035E-2</v>
+        <v>-3.3503681179227307E-2</v>
       </c>
       <c r="M4">
-        <v>-0.24633520647259943</v>
+        <v>-0.35612961410659494</v>
       </c>
       <c r="N4">
-        <v>92.143188970025463</v>
+        <v>94.278996701272078</v>
       </c>
       <c r="O4">
-        <v>55.956261828777663</v>
+        <v>87.122016951039342</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B5">
-        <v>1016.1563763732124</v>
+        <v>784.01810565250082</v>
       </c>
       <c r="C5">
-        <v>9590263817.7452202</v>
+        <v>9425216088.144846</v>
       </c>
       <c r="D5">
-        <v>9437783.4364175871</v>
+        <v>12021681.668053685</v>
       </c>
       <c r="E5">
-        <v>0.48212753794713165</v>
+        <v>0.6047268834892624</v>
       </c>
       <c r="F5">
-        <v>156.67901464721251</v>
+        <v>148.41216466318815</v>
       </c>
       <c r="G5">
-        <v>691.18216868878562</v>
+        <v>538.59795200090059</v>
       </c>
       <c r="H5">
-        <v>1.2101255825117465</v>
+        <v>-0.25272924176920852</v>
       </c>
       <c r="I5">
-        <v>-4.3310217984809829E-2</v>
+        <v>-4.9774400373029382E-2</v>
       </c>
       <c r="J5">
-        <v>-0.5671332934267298</v>
+        <v>0.27159478563925998</v>
       </c>
       <c r="K5">
-        <v>-0.50709841954439916</v>
+        <v>0.25213414892893815</v>
       </c>
       <c r="L5">
-        <v>8.302758032673685E-2</v>
+        <v>-8.2604403998122189E-2</v>
       </c>
       <c r="M5">
-        <v>1.2162320174033208</v>
+        <v>-0.24587929212811932</v>
       </c>
       <c r="N5">
-        <v>96.998860741023009</v>
+        <v>90.929185475562264</v>
       </c>
       <c r="O5">
-        <v>44.003095689306029</v>
+        <v>55.044226110144713</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B6">
-        <v>459.77313887221686</v>
+        <v>1049.1754120135931</v>
       </c>
       <c r="C6">
-        <v>10024423797.591002</v>
+        <v>9918924613.1075573</v>
       </c>
       <c r="D6">
-        <v>21802978.360545449</v>
+        <v>9454019.3179622926</v>
       </c>
       <c r="E6">
-        <v>0.97814159472057183</v>
+        <v>0.48295694515363163</v>
       </c>
       <c r="F6">
-        <v>144.66761280441656</v>
+        <v>161.77553643159669</v>
       </c>
       <c r="G6">
-        <v>311.87265740281964</v>
+        <v>714.20655390940976</v>
       </c>
       <c r="H6">
-        <v>-2.6066897717813564E-3</v>
+        <v>1.210617188802134</v>
       </c>
       <c r="I6">
-        <v>1.39008753360228E-2</v>
+        <v>-4.3077922640073374E-2</v>
       </c>
       <c r="J6">
-        <v>1.655070766819855E-2</v>
+        <v>-0.56712447446477454</v>
       </c>
       <c r="K6">
-        <v>1.0368208674844448E-2</v>
+        <v>-0.50708837746858282</v>
       </c>
       <c r="L6">
-        <v>5.754434254367613E-3</v>
+        <v>8.3696161698424421E-2</v>
       </c>
       <c r="M6">
-        <v>-1.6746158767168007E-3</v>
+        <v>1.2163174140894872</v>
       </c>
       <c r="N6">
-        <v>101.39008753360228</v>
+        <v>95.692207735992667</v>
       </c>
       <c r="O6">
-        <v>101.65507076681986</v>
+        <v>43.287552553522552</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B7">
-        <v>460.97475705648537</v>
+        <v>474.60746135883858</v>
       </c>
       <c r="C7">
-        <v>9886986037.2383537</v>
+        <v>10365446516.265041</v>
       </c>
       <c r="D7">
-        <v>21447998.802300699</v>
+        <v>21840041.213401809</v>
       </c>
       <c r="E7">
-        <v>0.9681040895016485</v>
+        <v>0.97980433626891994</v>
       </c>
       <c r="F7">
-        <v>143.83989558213406</v>
+        <v>149.2812673416262</v>
       </c>
       <c r="G7">
-        <v>312.3958003699388</v>
+        <v>322.2492181711354</v>
       </c>
       <c r="H7">
-        <v>-3.564570624302521E-2</v>
+        <v>-2.3237134232800827E-3</v>
       </c>
       <c r="I7">
-        <v>1.5666737236474715E-2</v>
+        <v>1.4159414678369009E-2</v>
       </c>
       <c r="J7">
-        <v>5.3209120145662148E-2</v>
+        <v>1.6521519378000837E-2</v>
       </c>
       <c r="K7">
-        <v>4.9247231921604406E-2</v>
+        <v>1.0339197903164399E-2</v>
       </c>
       <c r="L7">
-        <v>4.0143346826670978E-6</v>
+        <v>5.633255473421972E-3</v>
       </c>
       <c r="M7">
-        <v>-3.0183511783170802E-2</v>
+        <v>-1.2163576101731355E-3</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1435,9 +1435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>